<commit_message>
fix: do not add undesirable combinations explicitly
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -2163,122 +2163,122 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>'Irregular' Uranium Nozzles</t>
+          <t>Counterfeit Bypass Nozzles</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>7654</v>
+        <v>43365</v>
       </c>
       <c r="C25" s="8" t="n">
-        <v>0.9915945911155113</v>
+        <v>0.9833807750370418</v>
       </c>
       <c r="D25" s="9" t="n">
-        <v>0.8968164920806885</v>
+        <v/>
       </c>
       <c r="E25" s="9" t="n">
-        <v>1.198663949966431</v>
+        <v>1.186895608901978</v>
       </c>
       <c r="F25" s="9" t="n">
-        <v/>
+        <v>1.399099230766296</v>
       </c>
       <c r="G25" s="9" t="n">
-        <v>2.392059087753296</v>
+        <v>2.390497207641602</v>
       </c>
       <c r="H25" s="9" t="n">
-        <v/>
+        <v>1.597500085830688</v>
       </c>
       <c r="I25" s="9" t="n">
-        <v>0.5988374948501587</v>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="inlineStr">
         <is>
-          <t>Black Market Catalyst Combustion Unit</t>
+          <t>Unlicensed Plasma Pump</t>
         </is>
       </c>
       <c r="B26" s="10" t="n">
-        <v>73420</v>
+        <v>99810</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>0.9883555190844333</v>
+        <v>0.982681423365152</v>
       </c>
       <c r="D26" s="12" t="n">
-        <v>0.8975188732147217</v>
+        <v/>
       </c>
       <c r="E26" s="12" t="n">
-        <v>1.010028839111328</v>
+        <v>1.196157574653626</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v/>
+        <v>1.399902820587158</v>
       </c>
       <c r="G26" s="12" t="n">
-        <v>2.379708766937256</v>
+        <v>2.373293876647949</v>
       </c>
       <c r="H26" s="12" t="n">
-        <v/>
+        <v>1.584073066711426</v>
       </c>
       <c r="I26" s="12" t="n">
-        <v>0.5922553539276123</v>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Banned Bypass Combustion Unit</t>
+          <t>Suspect Plasma Nozzles</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>833</v>
+        <v>12637</v>
       </c>
       <c r="C27" s="8" t="n">
-        <v>0.9868339793892986</v>
+        <v>0.9813988107591365</v>
       </c>
       <c r="D27" s="9" t="n">
-        <v>0.8896762728691101</v>
+        <v/>
       </c>
       <c r="E27" s="9" t="n">
-        <v>1.199914455413818</v>
+        <v>1.195326447486877</v>
       </c>
       <c r="F27" s="9" t="n">
-        <v/>
+        <v>1.398698210716248</v>
       </c>
       <c r="G27" s="9" t="n">
-        <v>2.394743919372559</v>
+        <v>2.382678031921387</v>
       </c>
       <c r="H27" s="9" t="n">
-        <v/>
+        <v>1.589505076408386</v>
       </c>
       <c r="I27" s="9" t="n">
-        <v>0.5963813066482544</v>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="inlineStr">
         <is>
-          <t>Suspect Plasma Nozzles</t>
+          <t>Smuggled Plasma Nozzles</t>
         </is>
       </c>
       <c r="B28" s="10" t="n">
-        <v>12637</v>
+        <v>59596</v>
       </c>
       <c r="C28" s="11" t="n">
-        <v>0.9813988107591365</v>
+        <v>0.9800512343322856</v>
       </c>
       <c r="D28" s="12" t="n">
         <v/>
       </c>
       <c r="E28" s="12" t="n">
-        <v>1.195326447486877</v>
+        <v>1.195916652679443</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>1.398698210716248</v>
+        <v>1.393261432647705</v>
       </c>
       <c r="G28" s="12" t="n">
-        <v>2.382678031921387</v>
+        <v>2.38945198059082</v>
       </c>
       <c r="H28" s="12" t="n">
-        <v>1.589505076408386</v>
+        <v>1.586968898773193</v>
       </c>
       <c r="I28" s="12" t="n">
         <v/>
@@ -2287,29 +2287,29 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Smuggled Plasma Nozzles</t>
+          <t>Reverse-Engineered Catalyst Nozzles</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>59596</v>
+        <v>60161</v>
       </c>
       <c r="C29" s="8" t="n">
-        <v>0.9800512343322856</v>
+        <v>0.979919176759133</v>
       </c>
       <c r="D29" s="9" t="n">
         <v/>
       </c>
       <c r="E29" s="9" t="n">
-        <v>1.195916652679443</v>
+        <v>1.196140289306641</v>
       </c>
       <c r="F29" s="9" t="n">
-        <v>1.393261432647705</v>
+        <v>1.398817539215088</v>
       </c>
       <c r="G29" s="9" t="n">
-        <v>2.38945198059082</v>
+        <v>2.384821176528931</v>
       </c>
       <c r="H29" s="9" t="n">
-        <v>1.586968898773193</v>
+        <v>1.580602884292602</v>
       </c>
       <c r="I29" s="9" t="n">
         <v/>
@@ -2318,29 +2318,29 @@
     <row r="30">
       <c r="A30" s="10" t="inlineStr">
         <is>
-          <t>Reverse-Engineered Catalyst Nozzles</t>
+          <t>Reverse-Engineered Uranium Igniter</t>
         </is>
       </c>
       <c r="B30" s="10" t="n">
-        <v>60161</v>
+        <v>6062</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>0.979919176759133</v>
+        <v>0.979596580166356</v>
       </c>
       <c r="D30" s="12" t="n">
         <v/>
       </c>
       <c r="E30" s="12" t="n">
-        <v>1.196140289306641</v>
+        <v>1.19882869720459</v>
       </c>
       <c r="F30" s="12" t="n">
-        <v>1.398817539215088</v>
+        <v>1.391174554824829</v>
       </c>
       <c r="G30" s="12" t="n">
-        <v>2.384821176528931</v>
+        <v>2.374314785003662</v>
       </c>
       <c r="H30" s="12" t="n">
-        <v>1.580602884292602</v>
+        <v>1.582233428955078</v>
       </c>
       <c r="I30" s="12" t="n">
         <v/>
@@ -2640,60 +2640,60 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Gravity Diffuser</t>
+          <t>Supersonic Dynamo</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>32744</v>
+        <v>7012</v>
       </c>
       <c r="C41" s="8" t="n">
-        <v>0.9453357136930844</v>
+        <v>0.9392741450554096</v>
       </c>
       <c r="D41" s="9" t="n">
-        <v>0.8496825098991394</v>
+        <v/>
       </c>
       <c r="E41" s="9" t="n">
-        <v>1.140560865402222</v>
+        <v>1.149417161941528</v>
       </c>
       <c r="F41" s="9" t="n">
-        <v/>
+        <v>1.321295499801636</v>
       </c>
       <c r="G41" s="9" t="n">
-        <v>2.322496175765991</v>
+        <v>2.349802255630493</v>
       </c>
       <c r="H41" s="9" t="n">
-        <v/>
+        <v>1.480804562568665</v>
       </c>
       <c r="I41" s="9" t="n">
-        <v>0.4962849617004394</v>
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="17" t="inlineStr">
         <is>
-          <t>Supersonic Dynamo</t>
+          <t>Antimatter Diffuser</t>
         </is>
       </c>
       <c r="B42" s="17" t="n">
-        <v>7012</v>
+        <v>32027</v>
       </c>
       <c r="C42" s="18" t="n">
-        <v>0.9392741450554096</v>
+        <v>0.9010382045893818</v>
       </c>
       <c r="D42" s="19" t="n">
         <v/>
       </c>
       <c r="E42" s="19" t="n">
-        <v>1.149417161941528</v>
+        <v>1.144293785095215</v>
       </c>
       <c r="F42" s="19" t="n">
-        <v>1.321295499801636</v>
+        <v>1.347607493400574</v>
       </c>
       <c r="G42" s="19" t="n">
-        <v>2.349802255630493</v>
+        <v>2.299631118774414</v>
       </c>
       <c r="H42" s="19" t="n">
-        <v>1.480804562568665</v>
+        <v>1.465230584144593</v>
       </c>
       <c r="I42" s="19" t="n">
         <v/>
@@ -2702,29 +2702,29 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Antimatter Diffuser</t>
+          <t>Perfect Pump</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>32027</v>
+        <v>2197</v>
       </c>
       <c r="C43" s="8" t="n">
-        <v>0.9010382045893818</v>
+        <v>0.883701386682016</v>
       </c>
       <c r="D43" s="9" t="n">
         <v/>
       </c>
       <c r="E43" s="9" t="n">
-        <v>1.144293785095215</v>
+        <v>1.116093993186951</v>
       </c>
       <c r="F43" s="9" t="n">
-        <v>1.347607493400574</v>
+        <v>1.33493173122406</v>
       </c>
       <c r="G43" s="9" t="n">
-        <v>2.299631118774414</v>
+        <v>2.325201272964477</v>
       </c>
       <c r="H43" s="9" t="n">
-        <v>1.465230584144593</v>
+        <v>1.499154448509216</v>
       </c>
       <c r="I43" s="9" t="n">
         <v/>
@@ -8774,181 +8774,181 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Risky Vacuum Ionizer</t>
+          <t>'Modified' Optical Supercharger</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>31496</v>
+        <v>22731</v>
       </c>
       <c r="C35" s="8" t="n">
-        <v>0.9915720550049296</v>
+        <v>0.9714813559343236</v>
       </c>
       <c r="D35" s="9" t="n">
-        <v/>
+        <v>1.997263073921204</v>
       </c>
       <c r="E35" s="9" t="n">
         <v/>
       </c>
-      <c r="F35" s="9" t="n">
-        <v>9.991353988647459</v>
+      <c r="F35" s="13" t="n">
+        <v>9.999753952026367</v>
       </c>
       <c r="G35" s="9" t="n">
-        <v>4.963578224182129</v>
+        <v>4.711563110351562</v>
       </c>
       <c r="H35" s="9" t="n">
-        <v>1.190783023834228</v>
+        <v/>
       </c>
       <c r="I35" s="9" t="n">
-        <v>0.9457166194915771</v>
+        <v>0.9292096495628356</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="inlineStr">
         <is>
-          <t>Counterfeit Sonic Ionizer</t>
+          <t>Risky Vacuum Supercapacitor</t>
         </is>
       </c>
       <c r="B36" s="10" t="n">
-        <v>48471</v>
+        <v>8641</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>0.9870129862051564</v>
-      </c>
-      <c r="D36" s="12" t="n">
-        <v/>
+        <v>0.9584205563726248</v>
+      </c>
+      <c r="D36" s="13" t="n">
+        <v>1.999986410140991</v>
       </c>
       <c r="E36" s="12" t="n">
         <v/>
       </c>
       <c r="F36" s="12" t="n">
-        <v>9.950421333312988</v>
+        <v/>
       </c>
       <c r="G36" s="12" t="n">
-        <v>4.983292579650879</v>
+        <v>4.813843727111816</v>
       </c>
       <c r="H36" s="12" t="n">
-        <v>1.199262857437134</v>
+        <v>1.199539303779602</v>
       </c>
       <c r="I36" s="12" t="n">
-        <v>0.9279792308807372</v>
+        <v>0.92414790391922</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Illegal Optical Dielectrics</t>
+          <t>Counterfeit Isotropic Ionizer</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>47219</v>
+        <v>95336</v>
       </c>
       <c r="C37" s="8" t="n">
-        <v>0.9867998754466608</v>
+        <v>0.9424549474806732</v>
       </c>
       <c r="D37" s="9" t="n">
-        <v>1.982534646987915</v>
+        <v>1.964128375053406</v>
       </c>
       <c r="E37" s="9" t="n">
-        <v/>
+        <v>0.9893336892127992</v>
       </c>
       <c r="F37" s="9" t="n">
-        <v/>
+        <v>9.851539611816406</v>
       </c>
       <c r="G37" s="9" t="n">
-        <v>4.986440181732178</v>
+        <v>4.402585029602051</v>
       </c>
       <c r="H37" s="9" t="n">
-        <v>1.190734267234802</v>
+        <v/>
       </c>
       <c r="I37" s="9" t="n">
-        <v>0.9476107954978944</v>
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="10" t="inlineStr">
         <is>
-          <t>'Modified' Optical Supercharger</t>
+          <t>Pirate Isotropic Ionizer</t>
         </is>
       </c>
       <c r="B38" s="10" t="n">
-        <v>22731</v>
+        <v>42667</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>0.9714813559343236</v>
+        <v>0.9339977631438596</v>
       </c>
       <c r="D38" s="12" t="n">
-        <v>1.997263073921204</v>
+        <v>1.997737169265747</v>
       </c>
       <c r="E38" s="12" t="n">
         <v/>
       </c>
-      <c r="F38" s="13" t="n">
-        <v>9.999753952026367</v>
-      </c>
-      <c r="G38" s="12" t="n">
-        <v>4.711563110351562</v>
+      <c r="F38" s="12" t="n">
+        <v>9.07684326171875</v>
+      </c>
+      <c r="G38" s="13" t="n">
+        <v>4.999813079833984</v>
       </c>
       <c r="H38" s="12" t="n">
         <v/>
       </c>
       <c r="I38" s="12" t="n">
-        <v>0.9292096495628356</v>
+        <v>0.9345950484275818</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Risky Vacuum Supercapacitor</t>
+          <t>Smuggled Vacuum Energy Lattice</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>8641</v>
+        <v>96773</v>
       </c>
       <c r="C39" s="8" t="n">
-        <v>0.9584205563726248</v>
-      </c>
-      <c r="D39" s="13" t="n">
-        <v>1.999986410140991</v>
+        <v>0.9332166098882768</v>
+      </c>
+      <c r="D39" s="9" t="n">
+        <v>1.999041795730591</v>
       </c>
       <c r="E39" s="9" t="n">
-        <v/>
+        <v>0.8150184750556946</v>
       </c>
       <c r="F39" s="9" t="n">
-        <v/>
+        <v>9.973913192749023</v>
       </c>
       <c r="G39" s="9" t="n">
-        <v>4.813843727111816</v>
+        <v>4.982959270477295</v>
       </c>
       <c r="H39" s="9" t="n">
-        <v>1.199539303779602</v>
+        <v/>
       </c>
       <c r="I39" s="9" t="n">
-        <v>0.92414790391922</v>
+        <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="10" t="inlineStr">
         <is>
-          <t>Counterfeit Isotropic Ionizer</t>
+          <t>Illegal Optical Heat Sink</t>
         </is>
       </c>
       <c r="B40" s="10" t="n">
-        <v>95336</v>
+        <v>12163</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>0.9424549474806732</v>
+        <v>0.9305310367719752</v>
       </c>
       <c r="D40" s="12" t="n">
-        <v>1.964128375053406</v>
+        <v>1.997154712677002</v>
       </c>
       <c r="E40" s="12" t="n">
-        <v>0.9893336892127992</v>
+        <v>0.8165081143379211</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>9.851539611816406</v>
+        <v>9.973670959472656</v>
       </c>
       <c r="G40" s="12" t="n">
-        <v>4.402585029602051</v>
+        <v>4.941802024841309</v>
       </c>
       <c r="H40" s="12" t="n">
         <v/>
@@ -8960,57 +8960,57 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Pirate Isotropic Ionizer</t>
+          <t>Banned Optical Energy Lattice</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>42667</v>
+        <v>50260</v>
       </c>
       <c r="C41" s="8" t="n">
-        <v>0.9339977631438596</v>
+        <v>0.9290166780439651</v>
       </c>
       <c r="D41" s="9" t="n">
-        <v>1.997737169265747</v>
+        <v>1.957504391670227</v>
       </c>
       <c r="E41" s="9" t="n">
-        <v/>
+        <v>0.8226012587547302</v>
       </c>
       <c r="F41" s="9" t="n">
-        <v>9.07684326171875</v>
-      </c>
-      <c r="G41" s="13" t="n">
-        <v>4.999813079833984</v>
+        <v>9.973701477050779</v>
+      </c>
+      <c r="G41" s="9" t="n">
+        <v>4.953860282897949</v>
       </c>
       <c r="H41" s="9" t="n">
         <v/>
       </c>
       <c r="I41" s="9" t="n">
-        <v>0.9345950484275818</v>
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="10" t="inlineStr">
         <is>
-          <t>Smuggled Vacuum Energy Lattice</t>
+          <t>Counterfeit Sonic Supercapacitor</t>
         </is>
       </c>
       <c r="B42" s="10" t="n">
-        <v>96773</v>
+        <v>82343</v>
       </c>
       <c r="C42" s="11" t="n">
-        <v>0.9332166098882768</v>
+        <v>0.9280751117400738</v>
       </c>
       <c r="D42" s="12" t="n">
-        <v>1.999041795730591</v>
+        <v>1.974175453186035</v>
       </c>
       <c r="E42" s="12" t="n">
-        <v>0.8150184750556946</v>
+        <v>0.8193949460983276</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>9.973913192749023</v>
+        <v>9.959745407104492</v>
       </c>
       <c r="G42" s="12" t="n">
-        <v>4.982959270477295</v>
+        <v>4.942864418029785</v>
       </c>
       <c r="H42" s="12" t="n">
         <v/>
@@ -9022,26 +9022,26 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Illegal Optical Heat Sink</t>
+          <t>Forbidden Luminous Projectile Web</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>12163</v>
+        <v>14031</v>
       </c>
       <c r="C43" s="8" t="n">
-        <v>0.9305310367719752</v>
+        <v>0.9271991789645162</v>
       </c>
       <c r="D43" s="9" t="n">
-        <v>1.997154712677002</v>
+        <v>1.94858455657959</v>
       </c>
       <c r="E43" s="9" t="n">
-        <v>0.8165081143379211</v>
+        <v>0.8261331915855408</v>
       </c>
       <c r="F43" s="9" t="n">
-        <v>9.973670959472656</v>
+        <v>9.95370388031006</v>
       </c>
       <c r="G43" s="9" t="n">
-        <v>4.941802024841309</v>
+        <v>4.943439483642578</v>
       </c>
       <c r="H43" s="9" t="n">
         <v/>
@@ -9057,22 +9057,22 @@
         </is>
       </c>
       <c r="B44" s="10" t="n">
-        <v>50260</v>
+        <v>12934</v>
       </c>
       <c r="C44" s="11" t="n">
-        <v>0.9290166780439651</v>
+        <v>0.9260675546642344</v>
       </c>
       <c r="D44" s="12" t="n">
-        <v>1.957504391670227</v>
+        <v>1.937574863433838</v>
       </c>
       <c r="E44" s="12" t="n">
-        <v>0.8226012587547302</v>
+        <v>0.8116999864578247</v>
       </c>
       <c r="F44" s="12" t="n">
-        <v>9.973701477050779</v>
+        <v>9.994359970092772</v>
       </c>
       <c r="G44" s="12" t="n">
-        <v>4.953860282897949</v>
+        <v>4.981221199035645</v>
       </c>
       <c r="H44" s="12" t="n">
         <v/>
@@ -9084,26 +9084,26 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Counterfeit Sonic Supercapacitor</t>
+          <t>Reverse-Engineered Luminous Ion Cycler</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>82343</v>
+        <v>97599</v>
       </c>
       <c r="C45" s="8" t="n">
-        <v>0.9280751117400738</v>
+        <v>0.9242354529216104</v>
       </c>
       <c r="D45" s="9" t="n">
-        <v>1.974175453186035</v>
+        <v>1.978277206420898</v>
       </c>
       <c r="E45" s="9" t="n">
-        <v>0.8193949460983276</v>
+        <v>0.8254376649856567</v>
       </c>
       <c r="F45" s="9" t="n">
-        <v>9.959745407104492</v>
+        <v>9.88090991973877</v>
       </c>
       <c r="G45" s="9" t="n">
-        <v>4.942864418029785</v>
+        <v>4.924174785614014</v>
       </c>
       <c r="H45" s="9" t="n">
         <v/>
@@ -9115,26 +9115,26 @@
     <row r="46">
       <c r="A46" s="10" t="inlineStr">
         <is>
-          <t>Forbidden Luminous Projectile Web</t>
+          <t>Black Market Vacuum Supercharger</t>
         </is>
       </c>
       <c r="B46" s="10" t="n">
-        <v>14031</v>
+        <v>332</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>0.9271991789645162</v>
+        <v>0.9231649586363156</v>
       </c>
       <c r="D46" s="12" t="n">
-        <v>1.94858455657959</v>
+        <v>1.980265974998474</v>
       </c>
       <c r="E46" s="12" t="n">
-        <v>0.8261331915855408</v>
+        <v>0.8131895661354065</v>
       </c>
       <c r="F46" s="12" t="n">
-        <v>9.95370388031006</v>
+        <v>9.915326118469238</v>
       </c>
       <c r="G46" s="12" t="n">
-        <v>4.943439483642578</v>
+        <v>4.936666965484619</v>
       </c>
       <c r="H46" s="12" t="n">
         <v/>
@@ -9282,48 +9282,48 @@
     <row r="52">
       <c r="A52" s="17" t="inlineStr">
         <is>
-          <t>Elemental Projectile Web</t>
+          <t>Neutrino Heat Sink</t>
         </is>
       </c>
       <c r="B52" s="17" t="n">
-        <v>7012</v>
+        <v>82022</v>
       </c>
       <c r="C52" s="18" t="n">
-        <v>0.9899186383511338</v>
+        <v>0.9845646949873272</v>
       </c>
       <c r="D52" s="19" t="n">
-        <v/>
+        <v>1.969621419906616</v>
       </c>
       <c r="E52" s="20" t="n">
         <v>0.8500000238418579</v>
       </c>
-      <c r="F52" s="19" t="n">
-        <v/>
+      <c r="F52" s="20" t="n">
+        <v>8</v>
       </c>
       <c r="G52" s="19" t="n">
-        <v>3.994172334671021</v>
+        <v>3.983700752258301</v>
       </c>
       <c r="H52" s="19" t="n">
-        <v>1.14836859703064</v>
+        <v/>
       </c>
       <c r="I52" s="19" t="n">
-        <v>0.8994443416595459</v>
+        <v/>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Neutrino Heat Sink</t>
+          <t>Pugneum Energy Lattice</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>82022</v>
+        <v>78703</v>
       </c>
       <c r="C53" s="8" t="n">
-        <v>0.9845646949873272</v>
+        <v>0.9768048359876385</v>
       </c>
       <c r="D53" s="9" t="n">
-        <v>1.969621419906616</v>
+        <v>1.988918542861938</v>
       </c>
       <c r="E53" s="20" t="n">
         <v>0.8500000238418579</v>
@@ -9332,7 +9332,7 @@
         <v>8</v>
       </c>
       <c r="G53" s="9" t="n">
-        <v>3.983700752258301</v>
+        <v>3.941122055053711</v>
       </c>
       <c r="H53" s="9" t="n">
         <v/>
@@ -9344,17 +9344,17 @@
     <row r="54">
       <c r="A54" s="17" t="inlineStr">
         <is>
-          <t>Pugneum Energy Lattice</t>
+          <t>Ancient Projectile Web</t>
         </is>
       </c>
       <c r="B54" s="17" t="n">
-        <v>78703</v>
+        <v>26632</v>
       </c>
       <c r="C54" s="18" t="n">
-        <v>0.9768048359876385</v>
+        <v>0.9705645337693696</v>
       </c>
       <c r="D54" s="19" t="n">
-        <v>1.988918542861938</v>
+        <v>1.953988552093506</v>
       </c>
       <c r="E54" s="20" t="n">
         <v>0.8500000238418579</v>
@@ -9363,7 +9363,7 @@
         <v>8</v>
       </c>
       <c r="G54" s="19" t="n">
-        <v>3.941122055053711</v>
+        <v>3.957338809967041</v>
       </c>
       <c r="H54" s="19" t="n">
         <v/>
@@ -9375,17 +9375,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Ancient Projectile Web</t>
+          <t>Elemental Energy Lattice</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>26632</v>
+        <v>54170</v>
       </c>
       <c r="C55" s="8" t="n">
-        <v>0.9705645337693696</v>
+        <v>0.9683708031934626</v>
       </c>
       <c r="D55" s="9" t="n">
-        <v>1.953988552093506</v>
+        <v>1.924584150314331</v>
       </c>
       <c r="E55" s="20" t="n">
         <v>0.8500000238418579</v>
@@ -9394,7 +9394,7 @@
         <v>8</v>
       </c>
       <c r="G55" s="9" t="n">
-        <v>3.957338809967041</v>
+        <v>3.980167865753174</v>
       </c>
       <c r="H55" s="9" t="n">
         <v/>

</xml_diff>

<commit_message>
feat: add parquet files and language es-419 to all items
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -181,7 +181,12 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -197,13 +202,11 @@
     <xf numFmtId="164" fontId="0" fillId="10" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -570,7 +573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,7 +618,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The repository contains a collection of CSV files with values of stats for every procedural item in No Man's Sky. This includes mainly technology upgrades but also the products (artifacts in-game).</t>
+          <t>The repository contains a collection of files with values of stats for every procedural item in No Man's Sky. This includes mainly technology upgrades but also the products (treasures/artifacts in-game).</t>
         </is>
       </c>
     </row>
@@ -806,6 +809,11 @@
           <t>Starship (Regular), Hyperdrive</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Product, Exhibit Fossil Sample</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
@@ -1027,47 +1035,54 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>Freighter, Freighter Hyperdrive</t>
+          <t>Mech (Minotaur), Minotaur Flamethrower</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Freighter, Expedition Speed Control</t>
+          <t>Freighter, Freighter Hyperdrive</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Freighter, Expedition Efficiency Control</t>
+          <t>Freighter, Expedition Speed Control</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Freighter, Expedition Defenses Control</t>
+          <t>Freighter, Expedition Efficiency Control</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>Freighter, Expedition Trade Control</t>
+          <t>Freighter, Expedition Defenses Control</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>Freighter, Expedition Scientific Control</t>
+          <t>Freighter, Expedition Trade Control</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
+        <is>
+          <t>Freighter, Expedition Scientific Control</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="inlineStr">
         <is>
           <t>Freighter, Expedition Mining Control</t>
         </is>
@@ -1133,6 +1148,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A60" r:id="rId52"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A61" r:id="rId53"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A62" r:id="rId54"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A63" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1144,7 +1160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1152,11 +1168,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
+    <col width="33" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="7" customWidth="1" min="4" max="4"/>
-    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1583,10 +1599,31 @@
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
+      <c r="C40" s="4" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>Exhibit Fossil Sample (PROC_EXH)</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="53" t="inlineStr">
+        <is>
+          <t>This product is not yet available in game version 4.13 but was added in 5.50.</t>
+        </is>
+      </c>
+      <c r="C42" s="4" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="29">
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A41:C41"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -1598,11 +1635,13 @@
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A42:E42"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D29:E29"/>
@@ -1633,7 +1672,7 @@
   <cols>
     <col width="47" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="27" customWidth="1" min="4" max="4"/>
     <col width="21" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
@@ -1691,7 +1730,7 @@
         <v>47228</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>0.998896353359536</v>
+        <v>0.9988963533595359</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>109.8834156990051</v>
@@ -1710,7 +1749,7 @@
         <v>11762</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.9979518184156224</v>
+        <v>0.9979518184156223</v>
       </c>
       <c r="D4" s="12" t="n">
         <v>109.9468946456909</v>
@@ -1733,7 +1772,7 @@
         <v>70391</v>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.9977182559396888</v>
+        <v>0.9977182559396887</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>109.8862409591675</v>
@@ -1752,7 +1791,7 @@
         <v>53087</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.9649868971333264</v>
+        <v>0.9649868971333265</v>
       </c>
       <c r="D6" s="13" t="n">
         <v>109.9997162818909</v>
@@ -1828,7 +1867,7 @@
         <v>0.7237513046230898</v>
       </c>
       <c r="D10" s="19" t="n">
-        <v>99.99896287918092</v>
+        <v>99.99896287918091</v>
       </c>
       <c r="E10" s="20" t="n">
         <v>29.54715490341187</v>
@@ -1927,16 +1966,16 @@
         <v>0.9922761371684586</v>
       </c>
       <c r="D15" s="9" t="n">
-        <v>9.979081153869627</v>
+        <v>9.979081153869629</v>
       </c>
       <c r="E15" s="9" t="n">
         <v>9.948956966400146</v>
       </c>
       <c r="F15" s="9" t="n">
-        <v>9.936714172363279</v>
+        <v>9.936714172363281</v>
       </c>
       <c r="G15" s="9" t="n">
-        <v>9.856748580932615</v>
+        <v>9.856748580932617</v>
       </c>
     </row>
     <row r="16">
@@ -1949,16 +1988,16 @@
         <v>29711</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>0.9874481046105952</v>
+        <v>0.9874481046105951</v>
       </c>
       <c r="D16" s="12" t="n">
         <v>9.850132465362549</v>
       </c>
       <c r="E16" s="12" t="n">
-        <v>9.92335081100464</v>
+        <v>9.923350811004639</v>
       </c>
       <c r="F16" s="12" t="n">
-        <v>9.920990467071531</v>
+        <v>9.920990467071533</v>
       </c>
       <c r="G16" s="12" t="n">
         <v>9.853219985961914</v>
@@ -1976,10 +2015,10 @@
         <v>75173</v>
       </c>
       <c r="C17" s="8" t="n">
-        <v>0.9874408093207624</v>
+        <v>0.9874408093207623</v>
       </c>
       <c r="D17" s="9" t="n">
-        <v>9.959471225738524</v>
+        <v>9.959471225738525</v>
       </c>
       <c r="E17" s="9" t="n">
         <v>9.753680229187012</v>
@@ -1988,7 +2027,7 @@
         <v>9.912323951721191</v>
       </c>
       <c r="G17" s="9" t="n">
-        <v>9.921956062316896</v>
+        <v>9.921956062316895</v>
       </c>
     </row>
     <row r="18">
@@ -2028,7 +2067,7 @@
         <v>18702</v>
       </c>
       <c r="C19" s="8" t="n">
-        <v>0.948824485247042</v>
+        <v>0.9488244852470421</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>9.22544002532959</v>
@@ -2040,7 +2079,7 @@
         <v>9.446024894714355</v>
       </c>
       <c r="G19" s="13" t="n">
-        <v>9.999918937683104</v>
+        <v>9.999918937683105</v>
       </c>
     </row>
     <row r="20">
@@ -2053,7 +2092,7 @@
         <v>54591</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>0.9423709060292116</v>
+        <v>0.9423709060292117</v>
       </c>
       <c r="D20" s="12" t="n">
         <v>9.317576885223389</v>
@@ -2062,7 +2101,7 @@
         <v>9.999763965606689</v>
       </c>
       <c r="F20" s="12" t="n">
-        <v>9.706592559814451</v>
+        <v>9.706592559814453</v>
       </c>
       <c r="G20" s="12" t="n">
         <v>8.901000022888184</v>
@@ -2086,7 +2125,7 @@
         <v>8.935773372650146</v>
       </c>
       <c r="E21" s="23" t="n">
-        <v>9.186553955078123</v>
+        <v>9.186553955078125</v>
       </c>
       <c r="F21" s="25" t="n">
         <v>9.999895095825195</v>
@@ -2232,7 +2271,7 @@
         <v>60161</v>
       </c>
       <c r="C27" s="8" t="n">
-        <v>0.9843283954743708</v>
+        <v>0.9843283954743707</v>
       </c>
       <c r="D27" s="9" t="n">
         <v/>
@@ -2269,7 +2308,7 @@
         <v/>
       </c>
       <c r="E28" s="12" t="n">
-        <v>18.68956089019776</v>
+        <v>18.68956089019775</v>
       </c>
       <c r="F28" s="12" t="n">
         <v>39.90992307662964</v>
@@ -2294,7 +2333,7 @@
         <v>39999</v>
       </c>
       <c r="C29" s="8" t="n">
-        <v>0.9839996766573992</v>
+        <v>0.9839996766573993</v>
       </c>
       <c r="D29" s="9" t="n">
         <v/>
@@ -2306,7 +2345,7 @@
         <v>39.33722972869873</v>
       </c>
       <c r="G29" s="9" t="n">
-        <v>238.6954545974732</v>
+        <v>238.6954545974731</v>
       </c>
       <c r="H29" s="9" t="n">
         <v>59.64560508728027</v>
@@ -2325,7 +2364,7 @@
         <v>77869</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>0.9823976260622704</v>
+        <v>0.9823976260622705</v>
       </c>
       <c r="D30" s="12" t="n">
         <v/>
@@ -2467,7 +2506,7 @@
         <v>52.92842388153076</v>
       </c>
       <c r="I34" s="13" t="n">
-        <v>59.99941229820252</v>
+        <v>59.99941229820251</v>
       </c>
     </row>
     <row r="35">
@@ -2480,7 +2519,7 @@
         <v>94592</v>
       </c>
       <c r="C35" s="8" t="n">
-        <v>0.9095343385408416</v>
+        <v>0.9095343385408415</v>
       </c>
       <c r="D35" s="9" t="n">
         <v/>
@@ -2526,7 +2565,7 @@
         <v>239.9996280670166</v>
       </c>
       <c r="H36" s="12" t="n">
-        <v>56.6474199295044</v>
+        <v>56.64741992950439</v>
       </c>
       <c r="I36" s="12" t="n">
         <v/>
@@ -2576,22 +2615,22 @@
         <v>0.3138845783510787</v>
       </c>
       <c r="D38" s="13" t="n">
-        <v>29.99929785728454</v>
+        <v>29.99929785728455</v>
       </c>
       <c r="E38" s="12" t="n">
-        <v>9.225809574127195</v>
+        <v>9.225809574127197</v>
       </c>
       <c r="F38" s="12" t="n">
         <v/>
       </c>
       <c r="G38" s="12" t="n">
-        <v>130.9027433395385</v>
+        <v>130.9027433395386</v>
       </c>
       <c r="H38" s="12" t="n">
         <v/>
       </c>
       <c r="I38" s="12" t="n">
-        <v>22.11072742938996</v>
+        <v>22.11072742938995</v>
       </c>
     </row>
     <row r="39">
@@ -2610,7 +2649,7 @@
         <v/>
       </c>
       <c r="E39" s="9" t="n">
-        <v>19.56769227981568</v>
+        <v>19.56769227981567</v>
       </c>
       <c r="F39" s="13" t="n">
         <v>39.99977111816406</v>
@@ -2647,7 +2686,7 @@
         <v>7012</v>
       </c>
       <c r="C41" s="8" t="n">
-        <v>0.9425510224284492</v>
+        <v>0.9425510224284491</v>
       </c>
       <c r="D41" s="9" t="n">
         <v/>
@@ -2678,7 +2717,7 @@
         <v>2197</v>
       </c>
       <c r="C42" s="18" t="n">
-        <v>0.910669851982552</v>
+        <v>0.9106698519825521</v>
       </c>
       <c r="D42" s="20" t="n">
         <v/>
@@ -2690,7 +2729,7 @@
         <v>33.49317312240601</v>
       </c>
       <c r="G42" s="20" t="n">
-        <v>232.5201272964477</v>
+        <v>232.5201272964478</v>
       </c>
       <c r="H42" s="20" t="n">
         <v>49.91544485092163</v>
@@ -2786,7 +2825,7 @@
         <v>234.9997997283936</v>
       </c>
       <c r="H45" s="9" t="n">
-        <v>36.40283346176148</v>
+        <v>36.40283346176147</v>
       </c>
       <c r="I45" s="9" t="n">
         <v>40.0019109249115</v>
@@ -2988,7 +3027,7 @@
         <v>13129</v>
       </c>
       <c r="C54" s="11" t="n">
-        <v>0.9999944898669992</v>
+        <v>0.9999944898669993</v>
       </c>
       <c r="D54" s="13" t="n">
         <v>20</v>
@@ -3011,7 +3050,7 @@
         <v>39884</v>
       </c>
       <c r="C55" s="8" t="n">
-        <v>0.9999748600181844</v>
+        <v>0.9999748600181845</v>
       </c>
       <c r="D55" s="13" t="n">
         <v>20</v>
@@ -3053,7 +3092,7 @@
         <v>39397</v>
       </c>
       <c r="C57" s="8" t="n">
-        <v>0.9999687759129964</v>
+        <v>0.9999687759129963</v>
       </c>
       <c r="D57" s="13" t="n">
         <v>20</v>
@@ -3212,7 +3251,7 @@
         <v>86376</v>
       </c>
       <c r="C65" s="8" t="n">
-        <v>0.9910006081525105</v>
+        <v>0.9910006081525103</v>
       </c>
       <c r="D65" s="29" t="n">
         <v>20</v>
@@ -3336,7 +3375,7 @@
         <v>3850</v>
       </c>
       <c r="C69" s="8" t="n">
-        <v>0.9881172850151204</v>
+        <v>0.9881172850151203</v>
       </c>
       <c r="D69" s="29" t="n">
         <v>20</v>
@@ -3367,7 +3406,7 @@
         <v>3153</v>
       </c>
       <c r="C70" s="31" t="n">
-        <v>0.987979102017566</v>
+        <v>0.9879791020175661</v>
       </c>
       <c r="D70" s="29" t="n">
         <v>20</v>
@@ -3429,7 +3468,7 @@
         <v>53181</v>
       </c>
       <c r="C72" s="31" t="n">
-        <v>0.9872193519471508</v>
+        <v>0.9872193519471507</v>
       </c>
       <c r="D72" s="29" t="n">
         <v>20</v>
@@ -3460,7 +3499,7 @@
         <v>69716</v>
       </c>
       <c r="C73" s="8" t="n">
-        <v>0.9863774662172948</v>
+        <v>0.9863774662172949</v>
       </c>
       <c r="D73" s="29" t="n">
         <v>20</v>
@@ -3491,7 +3530,7 @@
         <v>71097</v>
       </c>
       <c r="C74" s="31" t="n">
-        <v>0.9512280592485844</v>
+        <v>0.9512280592485843</v>
       </c>
       <c r="D74" s="29" t="n">
         <v>20</v>
@@ -3562,7 +3601,7 @@
         <v>32.06693828105927</v>
       </c>
       <c r="F76" s="32" t="n">
-        <v>94.59738731384276</v>
+        <v>94.59738731384277</v>
       </c>
       <c r="G76" s="29" t="n">
         <v>74.99861717224121</v>
@@ -3615,7 +3654,7 @@
         <v>3260</v>
       </c>
       <c r="C78" s="31" t="n">
-        <v>0.3834075566738339</v>
+        <v>0.383407556673834</v>
       </c>
       <c r="D78" s="32" t="n">
         <v/>
@@ -3734,7 +3773,11 @@
       <c r="C84" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D84" s="16" t="inlineStr"/>
+      <c r="D84" s="37" t="inlineStr">
+        <is>
+          <t>This technology is outdated in game version 4.13 as it was changed in 5.50.</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3783,32 +3826,32 @@
         <v>18072</v>
       </c>
       <c r="C87" s="8" t="n">
-        <v>0.9999984740791832</v>
+        <v>0.9999984740791831</v>
       </c>
       <c r="D87" s="9" t="n">
         <v>179.9985504150391</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="37" t="inlineStr">
+      <c r="A88" s="38" t="inlineStr">
         <is>
           <t>Pure Oxygen Gas Pressurizer</t>
         </is>
       </c>
-      <c r="B88" s="37" t="n">
+      <c r="B88" s="38" t="n">
         <v>53523</v>
       </c>
-      <c r="C88" s="38" t="n">
-        <v>0.9999493394288784</v>
-      </c>
-      <c r="D88" s="39" t="n">
+      <c r="C88" s="39" t="n">
+        <v>0.9999493394288783</v>
+      </c>
+      <c r="D88" s="40" t="n">
         <v>179.99609375</v>
       </c>
-      <c r="E88" s="37" t="n"/>
-      <c r="F88" s="37" t="n"/>
-      <c r="G88" s="37" t="n"/>
-      <c r="H88" s="37" t="n"/>
-      <c r="I88" s="37" t="n"/>
+      <c r="E88" s="38" t="n"/>
+      <c r="F88" s="38" t="n"/>
+      <c r="G88" s="38" t="n"/>
+      <c r="H88" s="38" t="n"/>
+      <c r="I88" s="38" t="n"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -3882,7 +3925,7 @@
         <v>51119</v>
       </c>
       <c r="C93" s="18" t="n">
-        <v>0.994477988847006</v>
+        <v>0.9944779888470059</v>
       </c>
       <c r="D93" s="20" t="n">
         <v>19.950270652771</v>
@@ -3924,7 +3967,7 @@
         <v>31472</v>
       </c>
       <c r="C95" s="18" t="n">
-        <v>0.9197621136413664</v>
+        <v>0.9197621136413663</v>
       </c>
       <c r="D95" s="20" t="n">
         <v>13.2892370223999</v>
@@ -3947,7 +3990,7 @@
         <v>66946</v>
       </c>
       <c r="C96" s="22" t="n">
-        <v>0.1323911635222845</v>
+        <v>0.1323911635222846</v>
       </c>
       <c r="D96" s="24" t="n">
         <v>19.99990940093994</v>
@@ -4032,7 +4075,7 @@
         <v>51119</v>
       </c>
       <c r="C101" s="18" t="n">
-        <v>0.994477988847006</v>
+        <v>0.9944779888470059</v>
       </c>
       <c r="D101" s="20" t="n">
         <v>19.950270652771</v>
@@ -4074,7 +4117,7 @@
         <v>31472</v>
       </c>
       <c r="C103" s="18" t="n">
-        <v>0.9197621136413664</v>
+        <v>0.9197621136413663</v>
       </c>
       <c r="D103" s="20" t="n">
         <v>13.2892370223999</v>
@@ -4097,7 +4140,7 @@
         <v>66946</v>
       </c>
       <c r="C104" s="22" t="n">
-        <v>0.1323911635222845</v>
+        <v>0.1323911635222846</v>
       </c>
       <c r="D104" s="24" t="n">
         <v>19.99990940093994</v>
@@ -4182,7 +4225,7 @@
         <v>51119</v>
       </c>
       <c r="C109" s="18" t="n">
-        <v>0.994477988847006</v>
+        <v>0.9944779888470059</v>
       </c>
       <c r="D109" s="20" t="n">
         <v>19.950270652771</v>
@@ -4224,7 +4267,7 @@
         <v>31472</v>
       </c>
       <c r="C111" s="18" t="n">
-        <v>0.9197621136413664</v>
+        <v>0.9197621136413663</v>
       </c>
       <c r="D111" s="20" t="n">
         <v>13.2892370223999</v>
@@ -4247,7 +4290,7 @@
         <v>66946</v>
       </c>
       <c r="C112" s="22" t="n">
-        <v>0.1323911635222845</v>
+        <v>0.1323911635222846</v>
       </c>
       <c r="D112" s="24" t="n">
         <v>19.99990940093994</v>
@@ -4332,7 +4375,7 @@
         <v>51119</v>
       </c>
       <c r="C117" s="18" t="n">
-        <v>0.994477988847006</v>
+        <v>0.9944779888470059</v>
       </c>
       <c r="D117" s="20" t="n">
         <v>19.950270652771</v>
@@ -4374,7 +4417,7 @@
         <v>31472</v>
       </c>
       <c r="C119" s="18" t="n">
-        <v>0.9197621136413664</v>
+        <v>0.9197621136413663</v>
       </c>
       <c r="D119" s="20" t="n">
         <v>13.2892370223999</v>
@@ -4397,7 +4440,7 @@
         <v>66946</v>
       </c>
       <c r="C120" s="22" t="n">
-        <v>0.1323911635222845</v>
+        <v>0.1323911635222846</v>
       </c>
       <c r="D120" s="24" t="n">
         <v>19.99990940093994</v>
@@ -4450,7 +4493,7 @@
   <cols>
     <col width="43" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
@@ -4518,13 +4561,13 @@
         <v>31230</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>0.9950916164820336</v>
+        <v>0.9950916164820337</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>29.91313934326172</v>
       </c>
       <c r="E3" s="9" t="n">
-        <v>19.9536681175232</v>
+        <v>19.95366811752319</v>
       </c>
       <c r="F3" s="13" t="n">
         <v>1.006500005722046</v>
@@ -4570,7 +4613,7 @@
         <v>14611</v>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.9940928164115588</v>
+        <v>0.9940928164115587</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>29.98849153518677</v>
@@ -4598,7 +4641,7 @@
         <v>0.9920100637144504</v>
       </c>
       <c r="D6" s="12" t="n">
-        <v>29.85880374908448</v>
+        <v>29.85880374908447</v>
       </c>
       <c r="E6" s="12" t="n">
         <v>19.91122961044312</v>
@@ -4622,7 +4665,7 @@
         <v>14876</v>
       </c>
       <c r="C7" s="8" t="n">
-        <v>0.9288640718002372</v>
+        <v>0.9288640718002371</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>27.11620330810547</v>
@@ -4736,7 +4779,7 @@
         <v>27225</v>
       </c>
       <c r="C12" s="18" t="n">
-        <v>0.9958451430789876</v>
+        <v>0.9958451430789875</v>
       </c>
       <c r="D12" s="20" t="n">
         <v>24.9840259552002</v>
@@ -4763,7 +4806,7 @@
         <v>25299</v>
       </c>
       <c r="C13" s="8" t="n">
-        <v>0.993831860320304</v>
+        <v>0.9938318603203041</v>
       </c>
       <c r="D13" s="9" t="n">
         <v>24.91304874420166</v>
@@ -4885,7 +4928,7 @@
         <v>81742</v>
       </c>
       <c r="C19" s="8" t="n">
-        <v>0.993552149136934</v>
+        <v>0.9935521491369339</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>9.94187593460083</v>
@@ -4927,7 +4970,7 @@
         <v>91934</v>
       </c>
       <c r="C21" s="8" t="n">
-        <v>0.9920724987236484</v>
+        <v>0.9920724987236483</v>
       </c>
       <c r="D21" s="9" t="n">
         <v>9.974133968353271</v>
@@ -5127,7 +5170,7 @@
         <v>13129</v>
       </c>
       <c r="C32" s="11" t="n">
-        <v>0.9999942567458164</v>
+        <v>0.9999942567458165</v>
       </c>
       <c r="D32" s="12" t="n">
         <v>319.9977111816406</v>
@@ -5242,7 +5285,7 @@
         <v>39397</v>
       </c>
       <c r="C38" s="18" t="n">
-        <v>0.9999860611880164</v>
+        <v>0.9999860611880163</v>
       </c>
       <c r="D38" s="20" t="n">
         <v>264.9984130859375</v>
@@ -5379,10 +5422,10 @@
         <v>30611</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>0.9999682603610036</v>
+        <v>0.9999682603610037</v>
       </c>
       <c r="D46" s="12" t="n">
-        <v>0.2499926090240478</v>
+        <v>0.2499926090240479</v>
       </c>
       <c r="E46" s="10" t="n"/>
       <c r="F46" s="10" t="n"/>
@@ -5494,7 +5537,7 @@
         <v>3.477537631988525</v>
       </c>
       <c r="F52" s="9" t="n">
-        <v>2.581226825714112</v>
+        <v>2.581226825714111</v>
       </c>
     </row>
     <row r="53">
@@ -5510,7 +5553,7 @@
         <v>0.9967709473579988</v>
       </c>
       <c r="D53" s="12" t="n">
-        <v>31.98837280273437</v>
+        <v>31.98837280273438</v>
       </c>
       <c r="E53" s="12" t="n">
         <v>3.494453430175781</v>
@@ -5554,7 +5597,7 @@
         <v>3014</v>
       </c>
       <c r="C55" s="11" t="n">
-        <v>0.9822228064654144</v>
+        <v>0.9822228064654145</v>
       </c>
       <c r="D55" s="12" t="n">
         <v>31.6190185546875</v>
@@ -5601,7 +5644,7 @@
         <v>6091</v>
       </c>
       <c r="C57" s="11" t="n">
-        <v>0.9614775364311748</v>
+        <v>0.9614775364311747</v>
       </c>
       <c r="D57" s="12" t="n">
         <v>31.238037109375</v>
@@ -5610,7 +5653,7 @@
         <v>3.133487701416016</v>
       </c>
       <c r="F57" s="13" t="n">
-        <v>2.60000228881836</v>
+        <v>2.600002288818359</v>
       </c>
       <c r="G57" s="10" t="n"/>
       <c r="H57" s="10" t="n"/>
@@ -5641,7 +5684,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="19" t="n">
-        <v>27.99994850158692</v>
+        <v>27.99994850158691</v>
       </c>
       <c r="E59" s="19" t="n">
         <v>2.999997138977051</v>
@@ -5660,7 +5703,7 @@
         <v>55029</v>
       </c>
       <c r="C60" s="18" t="n">
-        <v>0.9999959035132144</v>
+        <v>0.9999959035132143</v>
       </c>
       <c r="D60" s="20" t="n">
         <v>27.99990844726562</v>
@@ -5698,18 +5741,18 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="37" t="inlineStr">
+      <c r="A62" s="38" t="inlineStr">
         <is>
           <t>Free Electron Refractor</t>
         </is>
       </c>
-      <c r="B62" s="37" t="n">
+      <c r="B62" s="38" t="n">
         <v>91149</v>
       </c>
-      <c r="C62" s="38" t="n">
+      <c r="C62" s="39" t="n">
         <v>0.9999765915040814</v>
       </c>
-      <c r="D62" s="39" t="n">
+      <c r="D62" s="40" t="n">
         <v>27.99971961975098</v>
       </c>
       <c r="E62" s="24" t="n">
@@ -5718,9 +5761,9 @@
       <c r="F62" s="24" t="n">
         <v>2.100002765655518</v>
       </c>
-      <c r="G62" s="37" t="n"/>
-      <c r="H62" s="37" t="n"/>
-      <c r="I62" s="37" t="n"/>
+      <c r="G62" s="38" t="n"/>
+      <c r="H62" s="38" t="n"/>
+      <c r="I62" s="38" t="n"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
@@ -5800,7 +5843,7 @@
         <v>79.78813171386719</v>
       </c>
       <c r="E67" s="12" t="n">
-        <v>99.95448589324953</v>
+        <v>99.95448589324951</v>
       </c>
       <c r="F67" s="10" t="n"/>
       <c r="G67" s="10" t="n"/>
@@ -5817,7 +5860,7 @@
         <v>70391</v>
       </c>
       <c r="C68" s="8" t="n">
-        <v>0.9979036313631016</v>
+        <v>0.9979036313631017</v>
       </c>
       <c r="D68" s="9" t="n">
         <v>79.80076599121094</v>
@@ -5865,7 +5908,7 @@
         <v>79.99617767333984</v>
       </c>
       <c r="E70" s="9" t="n">
-        <v>90.07599353790285</v>
+        <v>90.07599353790283</v>
       </c>
     </row>
     <row r="71">
@@ -5890,7 +5933,7 @@
         <v>66168</v>
       </c>
       <c r="C72" s="8" t="n">
-        <v>0.9980601415663476</v>
+        <v>0.9980601415663475</v>
       </c>
       <c r="D72" s="9" t="n">
         <v>69.97612762451172</v>
@@ -6031,7 +6074,7 @@
         <v>7.97822093963623</v>
       </c>
       <c r="E79" s="12" t="n">
-        <v>9.982490539550779</v>
+        <v>9.982490539550781</v>
       </c>
       <c r="F79" s="12" t="n">
         <v>9.969782829284668</v>
@@ -6056,7 +6099,7 @@
         <v>7.982386589050293</v>
       </c>
       <c r="E80" s="9" t="n">
-        <v>9.968090057373049</v>
+        <v>9.968090057373047</v>
       </c>
       <c r="F80" s="9" t="n">
         <v>9.966003894805908</v>
@@ -6072,7 +6115,7 @@
         <v>3014</v>
       </c>
       <c r="C81" s="11" t="n">
-        <v>0.981111412870158</v>
+        <v>0.9811114128701581</v>
       </c>
       <c r="D81" s="12" t="n">
         <v>7.904754638671875</v>
@@ -6097,7 +6140,7 @@
         <v>6091</v>
       </c>
       <c r="C82" s="8" t="n">
-        <v>0.9434718761907592</v>
+        <v>0.9434718761907591</v>
       </c>
       <c r="D82" s="9" t="n">
         <v>7.80950927734375</v>
@@ -6203,7 +6246,7 @@
         <v>95159</v>
       </c>
       <c r="C87" s="8" t="n">
-        <v>0.3904691919165446</v>
+        <v>0.3904691919165447</v>
       </c>
       <c r="D87" s="9" t="n">
         <v>6.000512599945068</v>
@@ -6216,29 +6259,29 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="37" t="inlineStr">
+      <c r="A88" s="38" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B88" s="37" t="n">
+      <c r="B88" s="38" t="n">
         <v>3014</v>
       </c>
-      <c r="C88" s="38" t="n">
+      <c r="C88" s="39" t="n">
         <v>0.2393532220868545</v>
       </c>
       <c r="D88" s="24" t="n">
         <v>7.999974250793457</v>
       </c>
-      <c r="E88" s="39" t="n">
+      <c r="E88" s="40" t="n">
         <v>6.08595609664917</v>
       </c>
-      <c r="F88" s="39" t="n">
+      <c r="F88" s="40" t="n">
         <v>6.003260612487793</v>
       </c>
-      <c r="G88" s="37" t="n"/>
-      <c r="H88" s="37" t="n"/>
-      <c r="I88" s="37" t="n"/>
+      <c r="G88" s="38" t="n"/>
+      <c r="H88" s="38" t="n"/>
+      <c r="I88" s="38" t="n"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -6298,7 +6341,7 @@
         <v>35510</v>
       </c>
       <c r="C92" s="8" t="n">
-        <v>0.9969819513033572</v>
+        <v>0.9969819513033573</v>
       </c>
       <c r="D92" s="9" t="n">
         <v>13.9401969909668</v>
@@ -6345,7 +6388,7 @@
         <v>43595</v>
       </c>
       <c r="C94" s="8" t="n">
-        <v>0.995461399457078</v>
+        <v>0.9954613994570779</v>
       </c>
       <c r="D94" s="9" t="n">
         <v>13.96477317810059</v>
@@ -6367,7 +6410,7 @@
         <v>3014</v>
       </c>
       <c r="C95" s="11" t="n">
-        <v>0.9752511195738712</v>
+        <v>0.9752511195738711</v>
       </c>
       <c r="D95" s="12" t="n">
         <v>13.80950927734375</v>
@@ -6451,7 +6494,7 @@
         <v>11278</v>
       </c>
       <c r="C99" s="8" t="n">
-        <v>0.9808057979513044</v>
+        <v>0.9808057979513045</v>
       </c>
       <c r="D99" s="9" t="n">
         <v>11.90246677398682</v>
@@ -6482,7 +6525,7 @@
         <v>8.999991416931152</v>
       </c>
       <c r="F100" s="20" t="n">
-        <v>9.614932537078856</v>
+        <v>9.614932537078857</v>
       </c>
       <c r="G100" s="17" t="n"/>
       <c r="H100" s="17" t="n"/>
@@ -6511,29 +6554,29 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="37" t="inlineStr">
+      <c r="A102" s="38" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B102" s="37" t="n">
+      <c r="B102" s="38" t="n">
         <v>3014</v>
       </c>
-      <c r="C102" s="38" t="n">
+      <c r="C102" s="39" t="n">
         <v>0.3009311425696053</v>
       </c>
       <c r="D102" s="24" t="n">
         <v>11.99998664855957</v>
       </c>
-      <c r="E102" s="39" t="n">
+      <c r="E102" s="40" t="n">
         <v>7.293200492858887</v>
       </c>
-      <c r="F102" s="39" t="n">
+      <c r="F102" s="40" t="n">
         <v>5.142772197723389</v>
       </c>
-      <c r="G102" s="37" t="n"/>
-      <c r="H102" s="37" t="n"/>
-      <c r="I102" s="37" t="n"/>
+      <c r="G102" s="38" t="n"/>
+      <c r="H102" s="38" t="n"/>
+      <c r="I102" s="38" t="n"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr"/>
@@ -6640,7 +6683,7 @@
         <v>43595</v>
       </c>
       <c r="C108" s="8" t="n">
-        <v>0.9955639574840384</v>
+        <v>0.9955639574840383</v>
       </c>
       <c r="D108" s="9" t="n">
         <v>13.96477317810059</v>
@@ -6687,13 +6730,13 @@
         <v>6091</v>
       </c>
       <c r="C110" s="8" t="n">
-        <v>0.9413384821088516</v>
+        <v>0.9413384821088515</v>
       </c>
       <c r="D110" s="9" t="n">
         <v>13.6190185546875</v>
       </c>
       <c r="E110" s="9" t="n">
-        <v>36.7660403251648</v>
+        <v>36.76604032516479</v>
       </c>
       <c r="F110" s="13" t="n">
         <v>19.99998092651367</v>
@@ -6709,7 +6752,7 @@
         <v>55029</v>
       </c>
       <c r="C111" s="11" t="n">
-        <v>0.265867307384741</v>
+        <v>0.2658673073847411</v>
       </c>
       <c r="D111" s="13" t="n">
         <v>13.99986457824707</v>
@@ -6806,29 +6849,29 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="37" t="inlineStr">
+      <c r="A116" s="38" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B116" s="37" t="n">
+      <c r="B116" s="38" t="n">
         <v>3014</v>
       </c>
-      <c r="C116" s="38" t="n">
-        <v>0.270063788528497</v>
+      <c r="C116" s="39" t="n">
+        <v>0.2700637885284971</v>
       </c>
       <c r="D116" s="24" t="n">
         <v>11.99998664855957</v>
       </c>
-      <c r="E116" s="39" t="n">
+      <c r="E116" s="40" t="n">
         <v>30.73297739028931</v>
       </c>
-      <c r="F116" s="39" t="n">
+      <c r="F116" s="40" t="n">
         <v>10.14277935028076</v>
       </c>
-      <c r="G116" s="37" t="n"/>
-      <c r="H116" s="37" t="n"/>
-      <c r="I116" s="37" t="n"/>
+      <c r="G116" s="38" t="n"/>
+      <c r="H116" s="38" t="n"/>
+      <c r="I116" s="38" t="n"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr"/>
@@ -6874,7 +6917,7 @@
   <cols>
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
@@ -6967,7 +7010,7 @@
         <v>27225</v>
       </c>
       <c r="C4" s="18" t="n">
-        <v>0.9958451430789876</v>
+        <v>0.9958451430789875</v>
       </c>
       <c r="D4" s="20" t="n">
         <v>24.9840259552002</v>
@@ -6994,7 +7037,7 @@
         <v>25299</v>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.993831860320304</v>
+        <v>0.9938318603203041</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>24.91304874420166</v>
@@ -7257,7 +7300,7 @@
         <v>39397</v>
       </c>
       <c r="C18" s="18" t="n">
-        <v>0.9999860611880164</v>
+        <v>0.9999860611880163</v>
       </c>
       <c r="D18" s="20" t="n">
         <v>264.9984130859375</v>
@@ -7299,7 +7342,7 @@
         <v>95566</v>
       </c>
       <c r="C20" s="18" t="n">
-        <v>0.9999615023288068</v>
+        <v>0.9999615023288069</v>
       </c>
       <c r="D20" s="20" t="n">
         <v>264.9972839355469</v>
@@ -7322,7 +7365,7 @@
         <v>19289</v>
       </c>
       <c r="C21" s="22" t="n">
-        <v>0.99990906584563</v>
+        <v>0.9999090658456301</v>
       </c>
       <c r="D21" s="23" t="n">
         <v>264.994873046875</v>
@@ -7459,7 +7502,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="19" t="n">
-        <v>27.99994850158692</v>
+        <v>27.99994850158691</v>
       </c>
       <c r="E29" s="19" t="n">
         <v>2.999997138977051</v>
@@ -7478,7 +7521,7 @@
         <v>55029</v>
       </c>
       <c r="C30" s="18" t="n">
-        <v>0.9999959035132144</v>
+        <v>0.9999959035132143</v>
       </c>
       <c r="D30" s="20" t="n">
         <v>27.99990844726562</v>
@@ -7550,7 +7593,7 @@
         <v>39397</v>
       </c>
       <c r="C33" s="8" t="n">
-        <v>0.999976396433282</v>
+        <v>0.9999763964332821</v>
       </c>
       <c r="D33" s="9" t="n">
         <v>27.99971771240234</v>
@@ -7563,18 +7606,18 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="37" t="inlineStr">
+      <c r="A34" s="38" t="inlineStr">
         <is>
           <t>Boundless Gills</t>
         </is>
       </c>
-      <c r="B34" s="37" t="n">
+      <c r="B34" s="38" t="n">
         <v>95566</v>
       </c>
-      <c r="C34" s="38" t="n">
+      <c r="C34" s="39" t="n">
         <v>0.9999561090701528</v>
       </c>
-      <c r="D34" s="39" t="n">
+      <c r="D34" s="40" t="n">
         <v>27.99951934814453</v>
       </c>
       <c r="E34" s="24" t="n">
@@ -7583,9 +7626,9 @@
       <c r="F34" s="24" t="n">
         <v>2.100002765655518</v>
       </c>
-      <c r="G34" s="37" t="n"/>
-      <c r="H34" s="37" t="n"/>
-      <c r="I34" s="37" t="n"/>
+      <c r="G34" s="38" t="n"/>
+      <c r="H34" s="38" t="n"/>
+      <c r="I34" s="38" t="n"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -7645,7 +7688,7 @@
         <v>49936</v>
       </c>
       <c r="C38" s="8" t="n">
-        <v>0.9966655828216964</v>
+        <v>0.9966655828216965</v>
       </c>
       <c r="D38" s="9" t="n">
         <v>69.97747802734375</v>
@@ -7667,7 +7710,7 @@
         <v>69684</v>
       </c>
       <c r="C39" s="18" t="n">
-        <v>0.9944162540760496</v>
+        <v>0.9944162540760497</v>
       </c>
       <c r="D39" s="20" t="n">
         <v>69.95756530761719</v>
@@ -7676,7 +7719,7 @@
         <v/>
       </c>
       <c r="F39" s="20" t="n">
-        <v>0.2980560660362243</v>
+        <v>0.2980560660362244</v>
       </c>
       <c r="G39" s="17" t="n"/>
       <c r="H39" s="17" t="n"/>
@@ -7692,7 +7735,7 @@
         <v>41731</v>
       </c>
       <c r="C40" s="8" t="n">
-        <v>0.9941467186673332</v>
+        <v>0.9941467186673333</v>
       </c>
       <c r="D40" s="9" t="n">
         <v/>
@@ -7714,7 +7757,7 @@
         <v>54394</v>
       </c>
       <c r="C41" s="18" t="n">
-        <v>0.9926566456291256</v>
+        <v>0.9926566456291257</v>
       </c>
       <c r="D41" s="20" t="n">
         <v>69.95663452148438</v>
@@ -7723,7 +7766,7 @@
         <v/>
       </c>
       <c r="F41" s="20" t="n">
-        <v>0.2962136566638946</v>
+        <v>0.2962136566638947</v>
       </c>
       <c r="G41" s="17" t="n"/>
       <c r="H41" s="17" t="n"/>
@@ -7786,7 +7829,7 @@
         <v>11278</v>
       </c>
       <c r="C44" s="8" t="n">
-        <v>0.9920887377651072</v>
+        <v>0.9920887377651073</v>
       </c>
       <c r="D44" s="9" t="n">
         <v>69.92576599121094</v>
@@ -7808,7 +7851,7 @@
         <v>37541</v>
       </c>
       <c r="C45" s="18" t="n">
-        <v>0.9914711364248509</v>
+        <v>0.9914711364248507</v>
       </c>
       <c r="D45" s="20" t="n">
         <v/>
@@ -7833,7 +7876,7 @@
         <v>50259</v>
       </c>
       <c r="C46" s="8" t="n">
-        <v>0.9913160081837884</v>
+        <v>0.9913160081837883</v>
       </c>
       <c r="D46" s="9" t="n">
         <v>69.99076843261719</v>
@@ -7861,7 +7904,7 @@
         <v/>
       </c>
       <c r="E47" s="19" t="n">
-        <v>94.99930143356325</v>
+        <v>94.99930143356323</v>
       </c>
       <c r="F47" s="20" t="n">
         <v>0.252625435590744</v>
@@ -7893,29 +7936,29 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="37" t="inlineStr">
+      <c r="A49" s="38" t="inlineStr">
         <is>
           <t>Vibrant Fluids</t>
         </is>
       </c>
-      <c r="B49" s="37" t="n">
+      <c r="B49" s="38" t="n">
         <v>96019</v>
       </c>
-      <c r="C49" s="38" t="n">
-        <v>0.0713635598800953</v>
-      </c>
-      <c r="D49" s="39" t="n">
-        <v/>
-      </c>
-      <c r="E49" s="39" t="n">
+      <c r="C49" s="39" t="n">
+        <v>0.07136355988009535</v>
+      </c>
+      <c r="D49" s="40" t="n">
+        <v/>
+      </c>
+      <c r="E49" s="40" t="n">
         <v>75.4543662071228</v>
       </c>
       <c r="F49" s="24" t="n">
         <v>0.299999475479126</v>
       </c>
-      <c r="G49" s="37" t="n"/>
-      <c r="H49" s="37" t="n"/>
-      <c r="I49" s="37" t="n"/>
+      <c r="G49" s="38" t="n"/>
+      <c r="H49" s="38" t="n"/>
+      <c r="I49" s="38" t="n"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -7949,7 +7992,7 @@
   <cols>
     <col width="48" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
@@ -8017,7 +8060,7 @@
         <v>50251</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>0.9267778723814536</v>
+        <v>0.9267778723814537</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>24.82168674468994</v>
@@ -8042,7 +8085,7 @@
         <v>43522</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>0.9117606877351256</v>
+        <v>0.9117606877351255</v>
       </c>
       <c r="D4" s="12" t="n">
         <v>24.99628067016602</v>
@@ -8173,7 +8216,7 @@
         <v>50653</v>
       </c>
       <c r="C9" s="8" t="n">
-        <v>0.3158447380651585</v>
+        <v>0.3158447380651586</v>
       </c>
       <c r="D9" s="9" t="n">
         <v/>
@@ -8213,7 +8256,7 @@
         <v>0.985101629656189</v>
       </c>
       <c r="D11" s="19" t="n">
-        <v>20.00000476837159</v>
+        <v>20.00000476837158</v>
       </c>
       <c r="E11" s="9" t="n">
         <v>49.79507923126221</v>
@@ -8235,10 +8278,10 @@
         <v>13919</v>
       </c>
       <c r="C12" s="18" t="n">
-        <v>0.9712307287221816</v>
+        <v>0.9712307287221815</v>
       </c>
       <c r="D12" s="19" t="n">
-        <v>20.00000476837159</v>
+        <v>20.00000476837158</v>
       </c>
       <c r="E12" s="20" t="n">
         <v>49.81646537780762</v>
@@ -8265,7 +8308,7 @@
         <v>0.7789028604200497</v>
       </c>
       <c r="D13" s="19" t="n">
-        <v>20.00000476837159</v>
+        <v>20.00000476837158</v>
       </c>
       <c r="E13" s="9" t="n">
         <v>49.80721473693848</v>
@@ -8290,7 +8333,7 @@
         <v>0.6916361316074581</v>
       </c>
       <c r="D14" s="19" t="n">
-        <v>20.00000476837159</v>
+        <v>20.00000476837158</v>
       </c>
       <c r="E14" s="20" t="n">
         <v>47.09628820419312</v>
@@ -8317,7 +8360,7 @@
         <v>0.5475210978208199</v>
       </c>
       <c r="D15" s="24" t="n">
-        <v>20.00000476837159</v>
+        <v>20.00000476837158</v>
       </c>
       <c r="E15" s="24" t="n">
         <v>49.99994039535522</v>
@@ -8394,7 +8437,7 @@
         <v>22629</v>
       </c>
       <c r="C19" s="8" t="n">
-        <v>0.9946783325763472</v>
+        <v>0.9946783325763473</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>10910.65139770508</v>
@@ -8504,13 +8547,13 @@
         <v>10999.97253417969</v>
       </c>
       <c r="E23" s="9" t="n">
-        <v>9973.393249511721</v>
+        <v>9973.393249511719</v>
       </c>
       <c r="F23" s="9" t="n">
         <v>10431.76651000977</v>
       </c>
       <c r="G23" s="9" t="n">
-        <v>47.99864292144776</v>
+        <v>47.99864292144775</v>
       </c>
     </row>
     <row r="24">
@@ -8523,7 +8566,7 @@
         <v>54591</v>
       </c>
       <c r="C24" s="11" t="n">
-        <v>0.9232787580234012</v>
+        <v>0.9232787580234013</v>
       </c>
       <c r="D24" s="12" t="n">
         <v>10241.748046875</v>
@@ -8587,19 +8630,19 @@
         <v>5820</v>
       </c>
       <c r="C27" s="8" t="n">
-        <v>0.9564421427673224</v>
+        <v>0.9564421427673225</v>
       </c>
       <c r="D27" s="9" t="n">
         <v>9940.318298339844</v>
       </c>
       <c r="E27" s="9" t="n">
-        <v>9617.481231689451</v>
+        <v>9617.481231689453</v>
       </c>
       <c r="F27" s="9" t="n">
         <v>9993.962097167969</v>
       </c>
       <c r="G27" s="9" t="n">
-        <v>31.14242553710937</v>
+        <v>31.14242553710938</v>
       </c>
     </row>
     <row r="28">
@@ -8781,16 +8824,16 @@
         <v>82949</v>
       </c>
       <c r="C35" s="8" t="n">
-        <v>0.9889454190365649</v>
+        <v>0.9889454190365647</v>
       </c>
       <c r="D35" s="9" t="n">
         <v>1.876828670501709</v>
       </c>
       <c r="E35" s="9" t="n">
-        <v>19.98597383499145</v>
+        <v>19.98597383499146</v>
       </c>
       <c r="F35" s="9" t="n">
-        <v>9.972799301147459</v>
+        <v>9.972799301147461</v>
       </c>
       <c r="G35" s="9" t="n">
         <v>4.914365768432617</v>
@@ -8812,7 +8855,7 @@
         <v>93848</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>0.9869612652434964</v>
+        <v>0.9869612652434965</v>
       </c>
       <c r="D36" s="12" t="n">
         <v>1.973940014839172</v>
@@ -8821,7 +8864,7 @@
         <v>19.8572039604187</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>9.926051139831545</v>
+        <v>9.926051139831543</v>
       </c>
       <c r="G36" s="12" t="n">
         <v>4.85235595703125</v>
@@ -8880,13 +8923,13 @@
         <v>1.855227589607239</v>
       </c>
       <c r="E38" s="12" t="n">
-        <v>19.96133923530578</v>
+        <v>19.96133923530579</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>9.835649490356444</v>
+        <v>9.835649490356445</v>
       </c>
       <c r="G38" s="12" t="n">
-        <v>4.987564086914063</v>
+        <v>4.987564086914062</v>
       </c>
       <c r="H38" s="12" t="n">
         <v/>
@@ -8905,7 +8948,7 @@
         <v>61864</v>
       </c>
       <c r="C39" s="8" t="n">
-        <v>0.9827493707773168</v>
+        <v>0.9827493707773169</v>
       </c>
       <c r="D39" s="9" t="n">
         <v>1.978936314582825</v>
@@ -8967,7 +9010,7 @@
         <v>59596</v>
       </c>
       <c r="C41" s="8" t="n">
-        <v>0.9801600262709956</v>
+        <v>0.9801600262709955</v>
       </c>
       <c r="D41" s="9" t="n">
         <v>1.916484713554382</v>
@@ -8976,7 +9019,7 @@
         <v>19.67199444770813</v>
       </c>
       <c r="F41" s="9" t="n">
-        <v>9.826056480407717</v>
+        <v>9.826056480407715</v>
       </c>
       <c r="G41" s="9" t="n">
         <v>4.994373321533203</v>
@@ -8998,7 +9041,7 @@
         <v>49362</v>
       </c>
       <c r="C42" s="11" t="n">
-        <v>0.9794837483009312</v>
+        <v>0.9794837483009311</v>
       </c>
       <c r="D42" s="12" t="n">
         <v>1.922943115234375</v>
@@ -9029,7 +9072,7 @@
         <v>16443</v>
       </c>
       <c r="C43" s="8" t="n">
-        <v>0.9792270282388532</v>
+        <v>0.9792270282388533</v>
       </c>
       <c r="D43" s="9" t="n">
         <v>1.963743209838867</v>
@@ -9038,7 +9081,7 @@
         <v>19.63067650794983</v>
       </c>
       <c r="F43" s="9" t="n">
-        <v>9.968592643737791</v>
+        <v>9.968592643737793</v>
       </c>
       <c r="G43" s="9" t="n">
         <v>4.798402309417725</v>
@@ -9060,7 +9103,7 @@
         <v>11470</v>
       </c>
       <c r="C44" s="11" t="n">
-        <v>0.9670315757066136</v>
+        <v>0.9670315757066137</v>
       </c>
       <c r="D44" s="12" t="n">
         <v>1.986700534820557</v>
@@ -9382,7 +9425,7 @@
         <v>26632</v>
       </c>
       <c r="C55" s="8" t="n">
-        <v>0.9705645337693696</v>
+        <v>0.9705645337693695</v>
       </c>
       <c r="D55" s="9" t="n">
         <v>1.953988552093506</v>
@@ -9624,7 +9667,7 @@
         <v>448.3980712890625</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>19.86939907073974</v>
+        <v>19.86939907073975</v>
       </c>
       <c r="G64" s="12" t="n">
         <v>399.0701198577881</v>
@@ -9642,7 +9685,7 @@
         <v>80565</v>
       </c>
       <c r="C65" s="8" t="n">
-        <v>0.9938359163261252</v>
+        <v>0.9938359163261253</v>
       </c>
       <c r="D65" s="9" t="n">
         <v/>
@@ -9654,7 +9697,7 @@
         <v>17.78464317321777</v>
       </c>
       <c r="G65" s="9" t="n">
-        <v>399.9524354934693</v>
+        <v>399.9524354934692</v>
       </c>
     </row>
     <row r="66">
@@ -9667,7 +9710,7 @@
         <v>94068</v>
       </c>
       <c r="C66" s="11" t="n">
-        <v>0.9934286837569772</v>
+        <v>0.9934286837569773</v>
       </c>
       <c r="D66" s="12" t="n">
         <v/>
@@ -9694,7 +9737,7 @@
         <v>8959</v>
       </c>
       <c r="C67" s="8" t="n">
-        <v>0.9933759959252888</v>
+        <v>0.9933759959252887</v>
       </c>
       <c r="D67" s="9" t="n">
         <v/>
@@ -9719,7 +9762,7 @@
         <v>29070</v>
       </c>
       <c r="C68" s="11" t="n">
-        <v>0.9931084465905272</v>
+        <v>0.9931084465905273</v>
       </c>
       <c r="D68" s="12" t="n">
         <v/>
@@ -9746,7 +9789,7 @@
         <v>16444</v>
       </c>
       <c r="C69" s="8" t="n">
-        <v>0.99292445619013</v>
+        <v>0.9929244561901301</v>
       </c>
       <c r="D69" s="9" t="n">
         <v/>
@@ -9771,7 +9814,7 @@
         <v>10548</v>
       </c>
       <c r="C70" s="11" t="n">
-        <v>0.9929219854277712</v>
+        <v>0.9929219854277713</v>
       </c>
       <c r="D70" s="12" t="n">
         <v/>
@@ -9798,7 +9841,7 @@
         <v>70034</v>
       </c>
       <c r="C71" s="8" t="n">
-        <v>0.9926445096533628</v>
+        <v>0.9926445096533627</v>
       </c>
       <c r="D71" s="9" t="n">
         <v/>
@@ -9829,7 +9872,7 @@
         <v/>
       </c>
       <c r="E72" s="12" t="n">
-        <v>430.0064086914063</v>
+        <v>430.0064086914062</v>
       </c>
       <c r="F72" s="12" t="n">
         <v>18.83049011230469</v>
@@ -9856,7 +9899,7 @@
         <v/>
       </c>
       <c r="E73" s="13" t="n">
-        <v>449.9907836914063</v>
+        <v>449.9907836914062</v>
       </c>
       <c r="F73" s="9" t="n">
         <v>19.38058137893677</v>
@@ -9875,7 +9918,7 @@
         <v>53087</v>
       </c>
       <c r="C74" s="11" t="n">
-        <v>0.9410597746196008</v>
+        <v>0.9410597746196009</v>
       </c>
       <c r="D74" s="13" t="n">
         <v>3.999991893768311</v>
@@ -9902,7 +9945,7 @@
         <v>76675</v>
       </c>
       <c r="C75" s="8" t="n">
-        <v>0.9141588276285152</v>
+        <v>0.9141588276285153</v>
       </c>
       <c r="D75" s="9" t="n">
         <v>3.645255565643311</v>
@@ -9945,7 +9988,7 @@
         <v/>
       </c>
       <c r="E77" s="9" t="n">
-        <v>399.2439575195313</v>
+        <v>399.2439575195312</v>
       </c>
       <c r="F77" s="9" t="n">
         <v>11.46901845932007</v>
@@ -9964,7 +10007,7 @@
         <v>68741</v>
       </c>
       <c r="C78" s="18" t="n">
-        <v>0.9598625578934804</v>
+        <v>0.9598625578934805</v>
       </c>
       <c r="D78" s="20" t="n">
         <v/>
@@ -9991,13 +10034,13 @@
         <v>65041</v>
       </c>
       <c r="C79" s="8" t="n">
-        <v>0.958512170718582</v>
+        <v>0.9585121707185821</v>
       </c>
       <c r="D79" s="9" t="n">
         <v/>
       </c>
       <c r="E79" s="9" t="n">
-        <v>399.7566528320313</v>
+        <v>399.7566528320312</v>
       </c>
       <c r="F79" s="9" t="n">
         <v>11.54352426528931</v>
@@ -10016,7 +10059,7 @@
         <v>3882</v>
       </c>
       <c r="C80" s="18" t="n">
-        <v>0.9515434248828344</v>
+        <v>0.9515434248828345</v>
       </c>
       <c r="D80" s="20" t="n">
         <v/>
@@ -10104,23 +10147,23 @@
         <v>357.3332824707031</v>
       </c>
       <c r="F83" s="19" t="n">
-        <v>14.99942541122436</v>
+        <v>14.99942541122437</v>
       </c>
       <c r="G83" s="9" t="n">
         <v/>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="40" t="inlineStr">
+      <c r="A84" s="41" t="inlineStr">
         <is>
           <t>Upgrade (1)</t>
         </is>
       </c>
-      <c r="B84" s="40" t="inlineStr"/>
-      <c r="C84" s="41" t="n">
+      <c r="B84" s="41" t="inlineStr"/>
+      <c r="C84" s="42" t="n">
         <v>2</v>
       </c>
-      <c r="D84" s="42" t="inlineStr"/>
+      <c r="D84" s="43" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -10134,7 +10177,7 @@
       <c r="C85" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D85" s="43" t="n">
+      <c r="D85" s="44" t="n">
         <v>1</v>
       </c>
       <c r="E85" s="9" t="n">
@@ -10143,36 +10186,36 @@
       <c r="F85" s="9" t="n">
         <v/>
       </c>
-      <c r="G85" s="43" t="n">
+      <c r="G85" s="44" t="n">
         <v>199.9960780143738</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="44" t="inlineStr">
+      <c r="A86" s="45" t="inlineStr">
         <is>
           <t>Tertiary Injector Plugs</t>
         </is>
       </c>
-      <c r="B86" s="44" t="n">
+      <c r="B86" s="45" t="n">
         <v>66503</v>
       </c>
-      <c r="C86" s="45" t="n">
+      <c r="C86" s="46" t="n">
         <v>0.9638186662144554</v>
       </c>
-      <c r="D86" s="46" t="n">
-        <v/>
-      </c>
-      <c r="E86" s="46" t="n">
+      <c r="D86" s="47" t="n">
+        <v/>
+      </c>
+      <c r="E86" s="47" t="n">
         <v>196.2135009765625</v>
       </c>
-      <c r="F86" s="46" t="n">
-        <v/>
-      </c>
-      <c r="G86" s="46" t="n">
+      <c r="F86" s="47" t="n">
+        <v/>
+      </c>
+      <c r="G86" s="47" t="n">
         <v>196.5467929840088</v>
       </c>
-      <c r="H86" s="44" t="n"/>
-      <c r="I86" s="44" t="n"/>
+      <c r="H86" s="45" t="n"/>
+      <c r="I86" s="45" t="n"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -10196,35 +10239,35 @@
         <v/>
       </c>
       <c r="G87" s="9" t="n">
-        <v>192.8195118904113</v>
+        <v>192.8195118904114</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="44" t="inlineStr">
+      <c r="A88" s="45" t="inlineStr">
         <is>
           <t>Efficient Coils</t>
         </is>
       </c>
-      <c r="B88" s="44" t="n">
+      <c r="B88" s="45" t="n">
         <v>38522</v>
       </c>
-      <c r="C88" s="45" t="n">
-        <v>0.9455232585792176</v>
-      </c>
-      <c r="D88" s="46" t="n">
-        <v/>
-      </c>
-      <c r="E88" s="46" t="n">
+      <c r="C88" s="46" t="n">
+        <v>0.9455232585792177</v>
+      </c>
+      <c r="D88" s="47" t="n">
+        <v/>
+      </c>
+      <c r="E88" s="47" t="n">
         <v>190.1379699707031</v>
       </c>
-      <c r="F88" s="46" t="n">
-        <v/>
-      </c>
-      <c r="G88" s="46" t="n">
+      <c r="F88" s="47" t="n">
+        <v/>
+      </c>
+      <c r="G88" s="47" t="n">
         <v>198.9651203155518</v>
       </c>
-      <c r="H88" s="44" t="n"/>
-      <c r="I88" s="44" t="n"/>
+      <c r="H88" s="45" t="n"/>
+      <c r="I88" s="45" t="n"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -10242,41 +10285,41 @@
         <v/>
       </c>
       <c r="E89" s="9" t="n">
-        <v>199.8390197753907</v>
+        <v>199.8390197753906</v>
       </c>
       <c r="F89" s="9" t="n">
         <v/>
       </c>
       <c r="G89" s="9" t="n">
-        <v>187.0068550109864</v>
+        <v>187.0068550109863</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="44" t="inlineStr">
+      <c r="A90" s="45" t="inlineStr">
         <is>
           <t>Lubricated Timing Loom</t>
         </is>
       </c>
-      <c r="B90" s="44" t="n">
+      <c r="B90" s="45" t="n">
         <v>81042</v>
       </c>
-      <c r="C90" s="45" t="n">
+      <c r="C90" s="46" t="n">
         <v>0.5</v>
       </c>
-      <c r="D90" s="46" t="n">
-        <v/>
-      </c>
-      <c r="E90" s="43" t="n">
+      <c r="D90" s="47" t="n">
+        <v/>
+      </c>
+      <c r="E90" s="44" t="n">
         <v>199.9966888427734</v>
       </c>
-      <c r="F90" s="46" t="n">
-        <v/>
-      </c>
-      <c r="G90" s="46" t="n">
-        <v/>
-      </c>
-      <c r="H90" s="44" t="n"/>
-      <c r="I90" s="44" t="n"/>
+      <c r="F90" s="47" t="n">
+        <v/>
+      </c>
+      <c r="G90" s="47" t="n">
+        <v/>
+      </c>
+      <c r="H90" s="45" t="n"/>
+      <c r="I90" s="45" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="21" t="inlineStr">
@@ -10296,7 +10339,7 @@
       <c r="E91" s="23" t="n">
         <v/>
       </c>
-      <c r="F91" s="47" t="n">
+      <c r="F91" s="48" t="n">
         <v>4.999732971191406</v>
       </c>
       <c r="G91" s="23" t="n">
@@ -10363,7 +10406,7 @@
         <v>39550</v>
       </c>
       <c r="C95" s="8" t="n">
-        <v>0.9995765225355084</v>
+        <v>0.9995765225355083</v>
       </c>
       <c r="D95" s="9" t="n">
         <v/>
@@ -10385,7 +10428,7 @@
         <v>28738</v>
       </c>
       <c r="C96" s="11" t="n">
-        <v>0.999479809794814</v>
+        <v>0.9994798097948141</v>
       </c>
       <c r="D96" s="12" t="n">
         <v>449.8092956542969</v>
@@ -10410,13 +10453,13 @@
         <v>54495</v>
       </c>
       <c r="C97" s="8" t="n">
-        <v>0.9992435063520884</v>
+        <v>0.9992435063520883</v>
       </c>
       <c r="D97" s="9" t="n">
         <v>449.8553771972656</v>
       </c>
       <c r="E97" s="9" t="n">
-        <v>59.83500480651856</v>
+        <v>59.83500480651855</v>
       </c>
       <c r="F97" s="9" t="n">
         <v/>
@@ -10432,7 +10475,7 @@
         <v>34103</v>
       </c>
       <c r="C98" s="11" t="n">
-        <v>0.9990004818269916</v>
+        <v>0.9990004818269917</v>
       </c>
       <c r="D98" s="12" t="n">
         <v>449.8304443359375</v>
@@ -10457,10 +10500,10 @@
         <v>38070</v>
       </c>
       <c r="C99" s="8" t="n">
-        <v>0.9987324878076376</v>
+        <v>0.9987324878076377</v>
       </c>
       <c r="D99" s="9" t="n">
-        <v>449.7459106445313</v>
+        <v>449.7459106445312</v>
       </c>
       <c r="E99" s="9" t="n">
         <v>59.74123477935791</v>
@@ -10488,7 +10531,7 @@
         <v>59.66074466705322</v>
       </c>
       <c r="F100" s="12" t="n">
-        <v>399.8524427413941</v>
+        <v>399.852442741394</v>
       </c>
       <c r="G100" s="10" t="n"/>
       <c r="H100" s="10" t="n"/>
@@ -10507,7 +10550,7 @@
         <v>0.9985063747078315</v>
       </c>
       <c r="D101" s="9" t="n">
-        <v>449.1589965820313</v>
+        <v>449.1589965820312</v>
       </c>
       <c r="E101" s="9" t="n">
         <v/>
@@ -10573,7 +10616,7 @@
         <v>3014</v>
       </c>
       <c r="C104" s="11" t="n">
-        <v>0.9914681405581628</v>
+        <v>0.9914681405581629</v>
       </c>
       <c r="D104" s="12" t="n">
         <v>444.4440002441406</v>
@@ -10598,7 +10641,7 @@
         <v>78682</v>
       </c>
       <c r="C105" s="8" t="n">
-        <v>0.9848508904625172</v>
+        <v>0.9848508904625171</v>
       </c>
       <c r="D105" s="13" t="n">
         <v>449.9908447265625</v>
@@ -10657,7 +10700,7 @@
         <v>22396</v>
       </c>
       <c r="C108" s="8" t="n">
-        <v>0.9962510291700516</v>
+        <v>0.9962510291700517</v>
       </c>
       <c r="D108" s="9" t="n">
         <v/>
@@ -10682,7 +10725,7 @@
         <v>0.9924501091511886</v>
       </c>
       <c r="D109" s="20" t="n">
-        <v>399.7300415039063</v>
+        <v>399.7300415039062</v>
       </c>
       <c r="E109" s="20" t="n">
         <v>49.82273578643799</v>
@@ -10764,29 +10807,29 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="37" t="inlineStr">
+      <c r="A113" s="38" t="inlineStr">
         <is>
           <t>Nano-Boosted Core</t>
         </is>
       </c>
-      <c r="B113" s="37" t="n">
+      <c r="B113" s="38" t="n">
         <v>96019</v>
       </c>
-      <c r="C113" s="38" t="n">
+      <c r="C113" s="39" t="n">
         <v>0.6721026498583409</v>
       </c>
-      <c r="D113" s="39" t="n">
+      <c r="D113" s="40" t="n">
         <v>351.1358947753906</v>
       </c>
-      <c r="E113" s="39" t="n">
+      <c r="E113" s="40" t="n">
         <v/>
       </c>
       <c r="F113" s="24" t="n">
         <v>299.9994516372681</v>
       </c>
-      <c r="G113" s="37" t="n"/>
-      <c r="H113" s="37" t="n"/>
-      <c r="I113" s="37" t="n"/>
+      <c r="G113" s="38" t="n"/>
+      <c r="H113" s="38" t="n"/>
+      <c r="I113" s="38" t="n"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr"/>
@@ -10841,7 +10884,7 @@
         <v>48726</v>
       </c>
       <c r="C117" s="8" t="n">
-        <v>0.986886723548118</v>
+        <v>0.9868867235481181</v>
       </c>
       <c r="D117" s="9" t="n">
         <v>24.39562082290649</v>
@@ -10860,7 +10903,7 @@
         <v>65202</v>
       </c>
       <c r="C118" s="11" t="n">
-        <v>0.9863880570562292</v>
+        <v>0.9863880570562293</v>
       </c>
       <c r="D118" s="12" t="n">
         <v>24.11457896232605</v>
@@ -10883,7 +10926,7 @@
         <v>36133</v>
       </c>
       <c r="C119" s="8" t="n">
-        <v>0.9805927518881792</v>
+        <v>0.9805927518881793</v>
       </c>
       <c r="D119" s="9" t="n">
         <v>24.20519590377808</v>
@@ -11084,7 +11127,7 @@
         <v>96621</v>
       </c>
       <c r="C129" s="8" t="n">
-        <v>0.9992763647179213</v>
+        <v>0.9992763647179211</v>
       </c>
       <c r="D129" s="13" t="n">
         <v>1</v>
@@ -11115,7 +11158,7 @@
         <v>98224</v>
       </c>
       <c r="C130" s="11" t="n">
-        <v>0.99465887475118</v>
+        <v>0.9946588747511799</v>
       </c>
       <c r="D130" s="13" t="n">
         <v>1</v>
@@ -11146,7 +11189,7 @@
         <v>45496</v>
       </c>
       <c r="C131" s="8" t="n">
-        <v>0.9935301466305504</v>
+        <v>0.9935301466305503</v>
       </c>
       <c r="D131" s="13" t="n">
         <v>1</v>
@@ -11177,7 +11220,7 @@
         <v>4195</v>
       </c>
       <c r="C132" s="11" t="n">
-        <v>0.9932690839332904</v>
+        <v>0.9932690839332903</v>
       </c>
       <c r="D132" s="13" t="n">
         <v>1</v>
@@ -11301,7 +11344,7 @@
         <v>48378</v>
       </c>
       <c r="C136" s="11" t="n">
-        <v>0.991410733833222</v>
+        <v>0.9914107338332219</v>
       </c>
       <c r="D136" s="13" t="n">
         <v>1</v>
@@ -11425,7 +11468,7 @@
         <v>11470</v>
       </c>
       <c r="C140" s="11" t="n">
-        <v>0.9609158400863336</v>
+        <v>0.9609158400863337</v>
       </c>
       <c r="D140" s="13" t="n">
         <v>1</v>
@@ -11592,7 +11635,7 @@
         <v>31871</v>
       </c>
       <c r="C146" s="18" t="n">
-        <v>0.9932524397422292</v>
+        <v>0.9932524397422291</v>
       </c>
       <c r="D146" s="19" t="n">
         <v>1</v>
@@ -11623,7 +11666,7 @@
         <v>39550</v>
       </c>
       <c r="C147" s="8" t="n">
-        <v>0.9911601917268412</v>
+        <v>0.9911601917268411</v>
       </c>
       <c r="D147" s="19" t="n">
         <v>1</v>
@@ -11654,7 +11697,7 @@
         <v>63898</v>
       </c>
       <c r="C148" s="18" t="n">
-        <v>0.9903265896524556</v>
+        <v>0.9903265896524555</v>
       </c>
       <c r="D148" s="19" t="n">
         <v>1</v>
@@ -11893,7 +11936,7 @@
         <v>71936</v>
       </c>
       <c r="C157" s="8" t="n">
-        <v>0.9932241335860768</v>
+        <v>0.9932241335860769</v>
       </c>
       <c r="D157" s="13" t="n">
         <v>12</v>
@@ -12022,13 +12065,13 @@
         <v>54591</v>
       </c>
       <c r="C162" s="11" t="n">
-        <v>0.9172722236421064</v>
+        <v>0.9172722236421063</v>
       </c>
       <c r="D162" s="13" t="n">
         <v>12</v>
       </c>
       <c r="E162" s="13" t="n">
-        <v>3.999920845031737</v>
+        <v>3.999920845031738</v>
       </c>
       <c r="F162" s="12" t="n">
         <v>18.55932474136353</v>
@@ -12095,10 +12138,10 @@
         <v>2.986183166503906</v>
       </c>
       <c r="F165" s="9" t="n">
-        <v>14.91845846176148</v>
+        <v>14.91845846176147</v>
       </c>
       <c r="G165" s="9" t="n">
-        <v>9.954744577407835</v>
+        <v>9.954744577407837</v>
       </c>
     </row>
     <row r="166">
@@ -12123,7 +12166,7 @@
         <v>14.95468616485596</v>
       </c>
       <c r="G166" s="20" t="n">
-        <v>9.958308935165403</v>
+        <v>9.958308935165405</v>
       </c>
       <c r="H166" s="17" t="n"/>
       <c r="I166" s="17" t="n"/>
@@ -12138,7 +12181,7 @@
         <v>96019</v>
       </c>
       <c r="C167" s="8" t="n">
-        <v>0.9787584450253992</v>
+        <v>0.9787584450253991</v>
       </c>
       <c r="D167" s="19" t="n">
         <v>12</v>
@@ -12150,7 +12193,7 @@
         <v>14.9999737739563</v>
       </c>
       <c r="G167" s="9" t="n">
-        <v>9.86270308494568</v>
+        <v>9.862703084945679</v>
       </c>
     </row>
     <row r="168">
@@ -12258,7 +12301,7 @@
       <c r="C172" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D172" s="48" t="inlineStr">
+      <c r="D172" s="37" t="inlineStr">
         <is>
           <t>This technology is outdated in game version 4.13 as it was changed in 4.30.</t>
         </is>
@@ -12360,7 +12403,7 @@
         <v>24.93092346191406</v>
       </c>
       <c r="F176" s="12" t="n">
-        <v>14.9219560623169</v>
+        <v>14.92195606231689</v>
       </c>
       <c r="G176" s="13" t="n">
         <v>1</v>
@@ -12381,7 +12424,7 @@
         <v>0.9733220428143452</v>
       </c>
       <c r="D177" s="9" t="n">
-        <v>24.2794156074524</v>
+        <v>24.27941560745239</v>
       </c>
       <c r="E177" s="9" t="n">
         <v>24.34797668457031</v>
@@ -12403,7 +12446,7 @@
         <v>76675</v>
       </c>
       <c r="C178" s="11" t="n">
-        <v>0.9667714239236096</v>
+        <v>0.9667714239236095</v>
       </c>
       <c r="D178" s="12" t="n">
         <v>24.23733472824097</v>
@@ -12455,7 +12498,7 @@
       <c r="C180" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D180" s="48" t="inlineStr">
+      <c r="D180" s="37" t="inlineStr">
         <is>
           <t>This technology is outdated in game version 4.13 as it was changed in 4.30.</t>
         </is>
@@ -12496,7 +12539,7 @@
         <v>17168</v>
       </c>
       <c r="C182" s="18" t="n">
-        <v>0.997039501230406</v>
+        <v>0.9970395012304059</v>
       </c>
       <c r="D182" s="20" t="n">
         <v>19.98088359832764</v>
@@ -12523,7 +12566,7 @@
         <v>48222</v>
       </c>
       <c r="C183" s="8" t="n">
-        <v>0.9946090680875224</v>
+        <v>0.9946090680875223</v>
       </c>
       <c r="D183" s="9" t="n">
         <v>19.91507411003113</v>
@@ -12548,7 +12591,7 @@
         <v>56209</v>
       </c>
       <c r="C184" s="18" t="n">
-        <v>0.9397970410949568</v>
+        <v>0.9397970410949567</v>
       </c>
       <c r="D184" s="19" t="n">
         <v>19.99955177307129</v>
@@ -12581,7 +12624,7 @@
         <v>11.55564785003662</v>
       </c>
       <c r="E185" s="24" t="n">
-        <v>24.99984741210937</v>
+        <v>24.99984741210938</v>
       </c>
       <c r="F185" s="24" t="n">
         <v>10</v>
@@ -12672,10 +12715,10 @@
         <v>6961</v>
       </c>
       <c r="C190" s="31" t="n">
-        <v>0.9901605496238128</v>
+        <v>0.9901605496238127</v>
       </c>
       <c r="D190" s="32" t="n">
-        <v>3.880991935729981</v>
+        <v>3.88099193572998</v>
       </c>
       <c r="E190" s="32" t="n">
         <v>19.97019052505493</v>
@@ -12719,7 +12762,7 @@
         <v>3014</v>
       </c>
       <c r="C192" s="31" t="n">
-        <v>0.9600351342820772</v>
+        <v>0.9600351342820773</v>
       </c>
       <c r="D192" s="32" t="n">
         <v>3.952377319335938</v>
@@ -12747,7 +12790,7 @@
         <v>0.6562913321285445</v>
       </c>
       <c r="D193" s="9" t="n">
-        <v>3.778197050094605</v>
+        <v>3.778197050094604</v>
       </c>
       <c r="E193" s="9" t="n">
         <v/>
@@ -12890,7 +12933,7 @@
         <v>41234</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>0.9822447613150236</v>
+        <v>0.9822447613150235</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>39.95621490478516</v>
@@ -12921,7 +12964,7 @@
         <v>19.9917733669281</v>
       </c>
       <c r="F4" s="20" t="n">
-        <v>9.707862138748167</v>
+        <v>9.707862138748169</v>
       </c>
       <c r="G4" s="17" t="n"/>
       <c r="H4" s="17" t="n"/>
@@ -12937,7 +12980,7 @@
         <v>36133</v>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.9686058437049916</v>
+        <v>0.9686058437049915</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>39.8820686340332</v>
@@ -12946,7 +12989,7 @@
         <v>19.80130076408386</v>
       </c>
       <c r="F5" s="9" t="n">
-        <v>9.781497716903688</v>
+        <v>9.781497716903687</v>
       </c>
     </row>
     <row r="6">
@@ -12997,29 +13040,29 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="37" t="inlineStr">
+      <c r="A8" s="38" t="inlineStr">
         <is>
           <t>Faultless Recycler</t>
         </is>
       </c>
-      <c r="B8" s="37" t="n">
+      <c r="B8" s="38" t="n">
         <v>32361</v>
       </c>
-      <c r="C8" s="38" t="n">
+      <c r="C8" s="39" t="n">
         <v>0.2099291858044448</v>
       </c>
-      <c r="D8" s="39" t="n">
+      <c r="D8" s="40" t="n">
         <v>30.36361312866211</v>
       </c>
-      <c r="E8" s="39" t="n">
+      <c r="E8" s="40" t="n">
         <v>15.00709652900696</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>9.999978542327881</v>
       </c>
-      <c r="G8" s="37" t="n"/>
-      <c r="H8" s="37" t="n"/>
-      <c r="I8" s="37" t="n"/>
+      <c r="G8" s="38" t="n"/>
+      <c r="H8" s="38" t="n"/>
+      <c r="I8" s="38" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -13074,7 +13117,7 @@
         <v>51119</v>
       </c>
       <c r="C12" s="8" t="n">
-        <v>0.994625922253674</v>
+        <v>0.9946259222536739</v>
       </c>
       <c r="D12" s="9" t="n">
         <v>39.94381713867188</v>
@@ -13099,7 +13142,7 @@
         <v>39.93930053710938</v>
       </c>
       <c r="E13" s="20" t="n">
-        <v>19.95298862457276</v>
+        <v>19.95298862457275</v>
       </c>
       <c r="F13" s="17" t="n"/>
       <c r="G13" s="17" t="n"/>
@@ -13243,7 +13286,7 @@
         <v>91149</v>
       </c>
       <c r="C21" s="18" t="n">
-        <v>0.9976217689972084</v>
+        <v>0.9976217689972083</v>
       </c>
       <c r="D21" s="20" t="n">
         <v>69.93979811668396</v>
@@ -13416,7 +13459,7 @@
         <v>4752</v>
       </c>
       <c r="C30" s="8" t="n">
-        <v>0.9912570715950052</v>
+        <v>0.9912570715950053</v>
       </c>
       <c r="D30" s="9" t="n">
         <v>19.95100378990173</v>
@@ -13501,7 +13544,7 @@
   <cols>
     <col width="33" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
@@ -13552,7 +13595,11 @@
       <c r="C2" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="inlineStr"/>
+      <c r="D2" s="37" t="inlineStr">
+        <is>
+          <t>This technology is outdated in game version 4.13 as it was changed in 5.50.</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -13586,7 +13633,7 @@
         <v>58006</v>
       </c>
       <c r="C4" s="18" t="n">
-        <v>0.9953973744231144</v>
+        <v>0.9953973744231143</v>
       </c>
       <c r="D4" s="20" t="n">
         <v>29.94859218597412</v>
@@ -13595,7 +13642,7 @@
         <v>10.00000238418579</v>
       </c>
       <c r="F4" s="20" t="n">
-        <v>29.95694279670716</v>
+        <v>29.95694279670715</v>
       </c>
       <c r="G4" s="17" t="n"/>
       <c r="H4" s="17" t="n"/>
@@ -13611,10 +13658,10 @@
         <v>5973</v>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.994895746926562</v>
+        <v>0.9948957469265621</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>29.92032170295716</v>
+        <v>29.92032170295715</v>
       </c>
       <c r="E5" s="19" t="n">
         <v>10.00000238418579</v>
@@ -13667,22 +13714,22 @@
         <v>10.00000238418579</v>
       </c>
       <c r="F7" s="9" t="n">
-        <v>26.8618792295456</v>
+        <v>26.86187922954559</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="37" t="inlineStr">
+      <c r="A8" s="38" t="inlineStr">
         <is>
           <t>High Pressure Turbine Controller</t>
         </is>
       </c>
-      <c r="B8" s="37" t="n">
+      <c r="B8" s="38" t="n">
         <v>96019</v>
       </c>
-      <c r="C8" s="38" t="n">
+      <c r="C8" s="39" t="n">
         <v>0.8061205041219637</v>
       </c>
-      <c r="D8" s="39" t="n">
+      <c r="D8" s="40" t="n">
         <v>25.81901550292969</v>
       </c>
       <c r="E8" s="24" t="n">
@@ -13691,9 +13738,9 @@
       <c r="F8" s="24" t="n">
         <v>29.99997437000275</v>
       </c>
-      <c r="G8" s="37" t="n"/>
-      <c r="H8" s="37" t="n"/>
-      <c r="I8" s="37" t="n"/>
+      <c r="G8" s="38" t="n"/>
+      <c r="H8" s="38" t="n"/>
+      <c r="I8" s="38" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -13767,13 +13814,13 @@
         <v>47825</v>
       </c>
       <c r="C13" s="18" t="n">
-        <v>0.9905774945793764</v>
+        <v>0.9905774945793763</v>
       </c>
       <c r="D13" s="20" t="n">
         <v>39.93930053710938</v>
       </c>
       <c r="E13" s="20" t="n">
-        <v>9.943854808807371</v>
+        <v>9.943854808807373</v>
       </c>
       <c r="F13" s="17" t="n"/>
       <c r="G13" s="17" t="n"/>
@@ -13838,7 +13885,7 @@
         <v>30.14566040039062</v>
       </c>
       <c r="E16" s="24" t="n">
-        <v>9.999948740005491</v>
+        <v>9.999948740005493</v>
       </c>
       <c r="F16" s="21" t="n"/>
       <c r="G16" s="21" t="n"/>
@@ -13863,7 +13910,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13871,7 +13918,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="33" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
@@ -13931,7 +13978,7 @@
         <v>51119</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>0.994625922253674</v>
+        <v>0.9946259222536739</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>39.94381713867188</v>
@@ -13956,7 +14003,7 @@
         <v>39.93930053710938</v>
       </c>
       <c r="E4" s="20" t="n">
-        <v>19.95298862457276</v>
+        <v>19.95298862457275</v>
       </c>
       <c r="F4" s="17" t="n"/>
       <c r="G4" s="17" t="n"/>
@@ -14108,7 +14155,7 @@
         <v>69520</v>
       </c>
       <c r="C12" s="18" t="n">
-        <v>0.9640559582925764</v>
+        <v>0.9640559582925765</v>
       </c>
       <c r="D12" s="20" t="n">
         <v>39.99628067016602</v>
@@ -14133,7 +14180,7 @@
         <v>94928</v>
       </c>
       <c r="C13" s="8" t="n">
-        <v>0.95926413915507</v>
+        <v>0.9592641391550701</v>
       </c>
       <c r="D13" s="9" t="n">
         <v>39.85224151611328</v>
@@ -14193,29 +14240,29 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="37" t="inlineStr">
+      <c r="A16" s="38" t="inlineStr">
         <is>
           <t>Faultless Recycler</t>
         </is>
       </c>
-      <c r="B16" s="37" t="n">
+      <c r="B16" s="38" t="n">
         <v>32361</v>
       </c>
-      <c r="C16" s="38" t="n">
+      <c r="C16" s="39" t="n">
         <v>0.2099282888068533</v>
       </c>
-      <c r="D16" s="39" t="n">
+      <c r="D16" s="40" t="n">
         <v>30.36361312866211</v>
       </c>
-      <c r="E16" s="39" t="n">
+      <c r="E16" s="40" t="n">
         <v>15.00709652900696</v>
       </c>
       <c r="F16" s="24" t="n">
         <v>9.999954700469971</v>
       </c>
-      <c r="G16" s="37" t="n"/>
-      <c r="H16" s="37" t="n"/>
-      <c r="I16" s="37" t="n"/>
+      <c r="G16" s="38" t="n"/>
+      <c r="H16" s="38" t="n"/>
+      <c r="I16" s="38" t="n"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -14312,10 +14359,10 @@
         <v>4752</v>
       </c>
       <c r="C22" s="8" t="n">
-        <v>0.9912579682294812</v>
+        <v>0.9912579682294811</v>
       </c>
       <c r="D22" s="9" t="n">
-        <v>29.96144294738769</v>
+        <v>29.9614429473877</v>
       </c>
       <c r="E22" s="9" t="n">
         <v>19.95100378990173</v>
@@ -14369,12 +14416,44 @@
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
+      <c r="C25" s="4" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="34" t="inlineStr">
+        <is>
+          <t>Minotaur Flamethrower (UP_MFIRE)</t>
+        </is>
+      </c>
+      <c r="B26" s="21" t="inlineStr">
+        <is>
+          <t>Seed</t>
+        </is>
+      </c>
+      <c r="C26" s="35" t="inlineStr">
+        <is>
+          <t>Perfection</t>
+        </is>
+      </c>
+      <c r="D26" s="36" t="inlineStr">
+        <is>
+          <t>This technology is not yet available in game version 4.13 but was added in 5.00.</t>
+        </is>
+      </c>
+      <c r="E26" s="21" t="n"/>
+      <c r="F26" s="21" t="n"/>
+      <c r="G26" s="21" t="n"/>
+      <c r="H26" s="21" t="n"/>
+      <c r="I26" s="21" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D19:I19"/>
     <mergeCell ref="D10:I10"/>
     <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D26:I26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -14473,7 +14552,7 @@
         <v>79741</v>
       </c>
       <c r="C4" s="18" t="n">
-        <v>0.9999991020547536</v>
+        <v>0.9999991020547535</v>
       </c>
       <c r="D4" s="20" t="n">
         <v>249.9985809326172</v>
@@ -14499,7 +14578,7 @@
         <v>0.9999985034245892</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>249.998550415039</v>
+        <v>249.9985504150391</v>
       </c>
       <c r="E5" s="19" t="n">
         <v>100</v>
@@ -14515,7 +14594,7 @@
         <v>81853</v>
       </c>
       <c r="C6" s="18" t="n">
-        <v>0.9999592931488256</v>
+        <v>0.9999592931488255</v>
       </c>
       <c r="D6" s="20" t="n">
         <v>249.9965515136719</v>
@@ -14541,7 +14620,7 @@
         <v>0.9999533068471822</v>
       </c>
       <c r="D7" s="23" t="n">
-        <v>249.9962463378907</v>
+        <v>249.9962463378906</v>
       </c>
       <c r="E7" s="24" t="n">
         <v>100</v>
@@ -14706,25 +14785,25 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="37" t="inlineStr">
+      <c r="A18" s="38" t="inlineStr">
         <is>
           <t>Navigation AI Unit from SS Emperor Bayaseb</t>
         </is>
       </c>
-      <c r="B18" s="37" t="n">
+      <c r="B18" s="38" t="n">
         <v>88814</v>
       </c>
-      <c r="C18" s="38" t="n">
+      <c r="C18" s="39" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="24" t="n">
         <v>19.9999988079071</v>
       </c>
-      <c r="E18" s="37" t="n"/>
-      <c r="F18" s="37" t="n"/>
-      <c r="G18" s="37" t="n"/>
-      <c r="H18" s="37" t="n"/>
-      <c r="I18" s="37" t="n"/>
+      <c r="E18" s="38" t="n"/>
+      <c r="F18" s="38" t="n"/>
+      <c r="G18" s="38" t="n"/>
+      <c r="H18" s="38" t="n"/>
+      <c r="I18" s="38" t="n"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>

</xml_diff>

<commit_message>
chore(game): update to 4.30
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -604,7 +604,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>4.13</t>
+          <t>4.30</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1612,7 @@
     <row r="42">
       <c r="A42" s="53" t="inlineStr">
         <is>
-          <t>This product is not yet available in game version 4.13 but was added in 5.50.</t>
+          <t>This product is not yet available in game version 4.30 but was added in 5.50.</t>
         </is>
       </c>
       <c r="C42" s="4" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="D81" s="36" t="inlineStr">
         <is>
-          <t>This technology is not yet available in game version 4.13 but was added in 4.40.</t>
+          <t>This technology is not yet available in game version 4.30 but was added in 4.40.</t>
         </is>
       </c>
       <c r="E81" s="21" t="n"/>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D84" s="37" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 4.13 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 4.30 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -7990,7 +7990,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="48" customWidth="1" min="1" max="1"/>
+    <col width="47" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
@@ -12303,30 +12303,30 @@
       </c>
       <c r="D172" s="37" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 4.13 as it was changed in 4.30.</t>
+          <t>This technology is outdated in game version 4.30 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Pirate Fine-Tuned Neutron Mirror</t>
+          <t>Counterfeit Advanced Safety Override</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>88056</v>
+        <v>29093</v>
       </c>
       <c r="C173" s="8" t="n">
-        <v>0.9928997897027326</v>
+        <v>0.9921309936703081</v>
       </c>
       <c r="D173" s="9" t="n">
-        <v>24.76871013641357</v>
+        <v>29.74483370780945</v>
       </c>
       <c r="E173" s="9" t="n">
-        <v>24.93540573120117</v>
+        <v>24.84856605529785</v>
       </c>
       <c r="F173" s="9" t="n">
-        <v>14.93302822113037</v>
+        <v>14.96304702758789</v>
       </c>
       <c r="G173" s="13" t="n">
         <v>1</v>
@@ -12335,23 +12335,23 @@
     <row r="174">
       <c r="A174" s="10" t="inlineStr">
         <is>
-          <t>Suspect Energised Plasma Unit</t>
+          <t>Outlawed Oscillating Ion Shaper</t>
         </is>
       </c>
       <c r="B174" s="10" t="n">
-        <v>52532</v>
+        <v>24640</v>
       </c>
       <c r="C174" s="11" t="n">
-        <v>0.9915487185848912</v>
+        <v>0.9920820889830231</v>
       </c>
       <c r="D174" s="12" t="n">
-        <v>24.78429675102234</v>
+        <v>29.67646718025208</v>
       </c>
       <c r="E174" s="12" t="n">
-        <v>24.79372024536133</v>
+        <v>24.94010734558105</v>
       </c>
       <c r="F174" s="12" t="n">
-        <v>14.98707103729248</v>
+        <v>14.93768119812012</v>
       </c>
       <c r="G174" s="13" t="n">
         <v>1</v>
@@ -12362,23 +12362,23 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Smuggled Oscillating Static Diffuser</t>
+          <t>Forbidden Advanced Linearity Warp</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>5873</v>
+        <v>6883</v>
       </c>
       <c r="C175" s="8" t="n">
-        <v>0.9906253887304816</v>
+        <v>0.9919042395788934</v>
       </c>
       <c r="D175" s="9" t="n">
-        <v>24.71501231193542</v>
+        <v>29.64625358581543</v>
       </c>
       <c r="E175" s="9" t="n">
-        <v>24.85857772827148</v>
+        <v>24.90845489501953</v>
       </c>
       <c r="F175" s="9" t="n">
-        <v>14.94597053527832</v>
+        <v>14.9869213104248</v>
       </c>
       <c r="G175" s="13" t="n">
         <v>1</v>
@@ -12387,23 +12387,23 @@
     <row r="176">
       <c r="A176" s="10" t="inlineStr">
         <is>
-          <t>Banned Advanced Positron Deflector</t>
+          <t>Banned Energised Plasma Unit</t>
         </is>
       </c>
       <c r="B176" s="10" t="n">
-        <v>70182</v>
+        <v>99050</v>
       </c>
       <c r="C176" s="11" t="n">
-        <v>0.9900756491816344</v>
+        <v>0.9916777469053119</v>
       </c>
       <c r="D176" s="12" t="n">
-        <v>24.63955283164978</v>
+        <v>29.70014810562134</v>
       </c>
       <c r="E176" s="12" t="n">
-        <v>24.93092346191406</v>
+        <v>24.86246871948242</v>
       </c>
       <c r="F176" s="12" t="n">
-        <v>14.92195606231689</v>
+        <v>14.96771430969238</v>
       </c>
       <c r="G176" s="13" t="n">
         <v>1</v>
@@ -12414,23 +12414,23 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Forbidden Advanced Antimatter Vent</t>
+          <t>Counterfeit Energised Plasma Unit</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>54591</v>
+        <v>14876</v>
       </c>
       <c r="C177" s="8" t="n">
-        <v>0.9733220428143452</v>
+        <v>0.980012780200203</v>
       </c>
       <c r="D177" s="9" t="n">
-        <v>24.27941560745239</v>
-      </c>
-      <c r="E177" s="9" t="n">
-        <v>24.34797668457031</v>
-      </c>
-      <c r="F177" s="13" t="n">
-        <v>14.99973678588867</v>
+        <v>29.41009998321533</v>
+      </c>
+      <c r="E177" s="13" t="n">
+        <v>24.99994087219238</v>
+      </c>
+      <c r="F177" s="9" t="n">
+        <v>14.4850606918335</v>
       </c>
       <c r="G177" s="13" t="n">
         <v>1</v>
@@ -12439,23 +12439,23 @@
     <row r="178">
       <c r="A178" s="10" t="inlineStr">
         <is>
-          <t>Reverse-Engineered Oscillating Compression Beam</t>
+          <t>Smuggled Polarised Antimatter Vent</t>
         </is>
       </c>
       <c r="B178" s="10" t="n">
-        <v>76675</v>
+        <v>4754</v>
       </c>
       <c r="C178" s="11" t="n">
-        <v>0.9667714239236095</v>
+        <v>0.9223657721378795</v>
       </c>
       <c r="D178" s="12" t="n">
-        <v>24.23733472824097</v>
-      </c>
-      <c r="E178" s="13" t="n">
-        <v>24.99976539611816</v>
-      </c>
-      <c r="F178" s="12" t="n">
-        <v>14.0961742401123</v>
+        <v>26.26911997795105</v>
+      </c>
+      <c r="E178" s="12" t="n">
+        <v>24.33263969421387</v>
+      </c>
+      <c r="F178" s="13" t="n">
+        <v>14.99974632263184</v>
       </c>
       <c r="G178" s="13" t="n">
         <v>1</v>
@@ -12466,23 +12466,23 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>'Modified' Advanced Neutron Mirror</t>
+          <t>Smuggled Polarised Neutron Mirror</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>74464</v>
+        <v>32361</v>
       </c>
       <c r="C179" s="8" t="n">
-        <v>0.6680914387446288</v>
+        <v>0.5924685549103823</v>
       </c>
       <c r="D179" s="13" t="n">
-        <v>24.99961256980896</v>
+        <v>29.99959588050842</v>
       </c>
       <c r="E179" s="9" t="n">
-        <v>18.01943969726562</v>
+        <v/>
       </c>
       <c r="F179" s="9" t="n">
-        <v>5.369376182556152</v>
+        <v>7.743895053863525</v>
       </c>
       <c r="G179" s="13" t="n">
         <v>1</v>
@@ -12498,32 +12498,28 @@
       <c r="C180" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D180" s="37" t="inlineStr">
-        <is>
-          <t>This technology is outdated in game version 4.13 as it was changed in 4.30.</t>
-        </is>
-      </c>
+      <c r="D180" s="16" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Vectorised Linearity Warp</t>
+          <t>Asymmetric Neutron Mirror</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>2250</v>
+        <v>69520</v>
       </c>
       <c r="C181" s="8" t="n">
-        <v>0.997698072468263</v>
+        <v>0.9917612699609807</v>
       </c>
       <c r="D181" s="9" t="n">
-        <v>19.98560428619385</v>
+        <v>49.96709823608398</v>
       </c>
       <c r="E181" s="9" t="n">
-        <v>24.97618675231934</v>
-      </c>
-      <c r="F181" s="19" t="n">
-        <v>10</v>
+        <v>24.99814033508301</v>
+      </c>
+      <c r="F181" s="9" t="n">
+        <v>17.78390884399414</v>
       </c>
       <c r="G181" s="19" t="n">
         <v>1</v>
@@ -12532,23 +12528,23 @@
     <row r="182">
       <c r="A182" s="17" t="inlineStr">
         <is>
-          <t>Supercooled Linearity Warp</t>
+          <t>Supreme Linearity Warp</t>
         </is>
       </c>
       <c r="B182" s="17" t="n">
-        <v>17168</v>
+        <v>40956</v>
       </c>
       <c r="C182" s="18" t="n">
-        <v>0.9970395012304059</v>
+        <v>0.9764194087793475</v>
       </c>
       <c r="D182" s="20" t="n">
-        <v>19.98088359832764</v>
+        <v>49.45964813232422</v>
       </c>
       <c r="E182" s="20" t="n">
-        <v>24.9700870513916</v>
-      </c>
-      <c r="F182" s="19" t="n">
-        <v>10</v>
+        <v>24.87591552734375</v>
+      </c>
+      <c r="F182" s="20" t="n">
+        <v>17.90608215332031</v>
       </c>
       <c r="G182" s="19" t="n">
         <v>1</v>
@@ -12559,23 +12555,23 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Asymmetric Positron Deflector</t>
+          <t>Supreme Antimatter Vent</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>48222</v>
+        <v>96019</v>
       </c>
       <c r="C183" s="8" t="n">
-        <v>0.9946090680875223</v>
+        <v>0.8195696577905798</v>
       </c>
       <c r="D183" s="9" t="n">
-        <v>19.91507411003113</v>
+        <v>44.42535638809204</v>
       </c>
       <c r="E183" s="9" t="n">
-        <v>24.9919319152832</v>
+        <v>24.61492919921875</v>
       </c>
       <c r="F183" s="19" t="n">
-        <v>10</v>
+        <v>17.99996757507324</v>
       </c>
       <c r="G183" s="19" t="n">
         <v>1</v>
@@ -12584,23 +12580,23 @@
     <row r="184">
       <c r="A184" s="17" t="inlineStr">
         <is>
-          <t>Supercooled Plasma Unit</t>
+          <t>Supercooled Safety Override</t>
         </is>
       </c>
       <c r="B184" s="17" t="n">
-        <v>56209</v>
+        <v>46775</v>
       </c>
       <c r="C184" s="18" t="n">
-        <v>0.9397970410949567</v>
+        <v>0.7431613738504467</v>
       </c>
       <c r="D184" s="19" t="n">
-        <v>19.99955177307129</v>
+        <v>49.99956488609314</v>
       </c>
       <c r="E184" s="20" t="n">
-        <v>24.04666900634766</v>
-      </c>
-      <c r="F184" s="19" t="n">
-        <v>10</v>
+        <v>20.29521751403809</v>
+      </c>
+      <c r="F184" s="20" t="n">
+        <v>15.13409805297852</v>
       </c>
       <c r="G184" s="19" t="n">
         <v>1</v>
@@ -12611,23 +12607,23 @@
     <row r="185">
       <c r="A185" s="21" t="inlineStr">
         <is>
-          <t>Vectorised Antimatter Vent</t>
+          <t>Supreme Neutron Mirror</t>
         </is>
       </c>
       <c r="B185" s="21" t="n">
-        <v>56579</v>
+        <v>3014</v>
       </c>
       <c r="C185" s="22" t="n">
-        <v>0.5111248813048657</v>
+        <v>0.6234213328274102</v>
       </c>
       <c r="D185" s="23" t="n">
-        <v>11.55564785003662</v>
+        <v>43.81182789802551</v>
       </c>
       <c r="E185" s="24" t="n">
-        <v>24.99984741210938</v>
-      </c>
-      <c r="F185" s="24" t="n">
-        <v>10</v>
+        <v>24.99996757507324</v>
+      </c>
+      <c r="F185" s="23" t="n">
+        <v>12.27174282073975</v>
       </c>
       <c r="G185" s="24" t="n">
         <v>1</v>
@@ -13597,7 +13593,7 @@
       </c>
       <c r="D2" s="37" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 4.13 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 4.30 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -14436,7 +14432,7 @@
       </c>
       <c r="D26" s="36" t="inlineStr">
         <is>
-          <t>This technology is not yet available in game version 4.13 but was added in 5.00.</t>
+          <t>This technology is not yet available in game version 4.30 but was added in 5.00.</t>
         </is>
       </c>
       <c r="E26" s="21" t="n"/>

</xml_diff>

<commit_message>
chore(game): update to 4.40
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -179,11 +179,6 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -205,6 +200,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -604,7 +604,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>4.30</t>
+          <t>4.40</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1612,7 @@
     <row r="42">
       <c r="A42" s="53" t="inlineStr">
         <is>
-          <t>This product is not yet available in game version 4.30 but was added in 5.50.</t>
+          <t>This product is not yet available in game version 4.40 but was added in 5.50.</t>
         </is>
       </c>
       <c r="C42" s="4" t="n"/>
@@ -1662,7 +1662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3711,447 +3711,644 @@
       <c r="C80" s="4" t="n"/>
     </row>
     <row r="81">
-      <c r="A81" s="34" t="inlineStr">
+      <c r="A81" s="1" t="inlineStr">
         <is>
           <t>Rebuilt Exosuit Module (UP_RBSUIT)</t>
         </is>
       </c>
-      <c r="B81" s="21" t="inlineStr">
+      <c r="B81" t="inlineStr">
         <is>
           <t>Seed</t>
         </is>
       </c>
-      <c r="C81" s="35" t="inlineStr">
+      <c r="C81" s="4" t="inlineStr">
         <is>
           <t>Perfection</t>
         </is>
       </c>
-      <c r="D81" s="36" t="inlineStr">
-        <is>
-          <t>This technology is not yet available in game version 4.30 but was added in 4.40.</t>
-        </is>
-      </c>
-      <c r="E81" s="21" t="n"/>
-      <c r="F81" s="21" t="n"/>
-      <c r="G81" s="21" t="n"/>
-      <c r="H81" s="21" t="n"/>
-      <c r="I81" s="21" t="n"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Core Health</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Shield Strength</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Life Support Tanks</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Solar Panel Power</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Fuel Efficiency</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Sprint Distance</t>
+        </is>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr"/>
-      <c r="C82" s="4" t="n"/>
+      <c r="A82" s="26" t="inlineStr">
+        <is>
+          <t>Salvaged Upgrade (!)</t>
+        </is>
+      </c>
+      <c r="B82" s="26" t="inlineStr"/>
+      <c r="C82" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D82" s="28" t="inlineStr"/>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Aeration Membrane (UP_UNW)</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Seed</t>
-        </is>
-      </c>
-      <c r="C83" s="4" t="inlineStr">
-        <is>
-          <t>Perfection</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Oxygen Tank</t>
-        </is>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Rusted Stasis Tank</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>86376</v>
+      </c>
+      <c r="C83" s="8" t="n">
+        <v>0.9910006081525103</v>
+      </c>
+      <c r="D83" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E83" s="9" t="n">
+        <v>34.13573205471039</v>
+      </c>
+      <c r="F83" s="9" t="n">
+        <v/>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>74.58446025848389</v>
+      </c>
+      <c r="H83" s="9" t="n">
+        <v/>
+      </c>
+      <c r="I83" s="9" t="n">
+        <v>59.94253158569336</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="14" t="inlineStr">
-        <is>
-          <t>Supreme Upgrade (3)</t>
-        </is>
-      </c>
-      <c r="B84" s="14" t="inlineStr"/>
-      <c r="C84" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D84" s="37" t="inlineStr">
-        <is>
-          <t>This technology is outdated in game version 4.30 as it was changed in 5.50.</t>
-        </is>
+      <c r="A84" s="30" t="inlineStr">
+        <is>
+          <t>Altered De-limiter</t>
+        </is>
+      </c>
+      <c r="B84" s="30" t="n">
+        <v>35295</v>
+      </c>
+      <c r="C84" s="31" t="n">
+        <v>0.9901543729762218</v>
+      </c>
+      <c r="D84" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E84" s="32" t="n">
+        <v/>
+      </c>
+      <c r="F84" s="32" t="n">
+        <v>109.7828269004822</v>
+      </c>
+      <c r="G84" s="32" t="n">
+        <v>73.64826202392578</v>
+      </c>
+      <c r="H84" s="32" t="n">
+        <v/>
+      </c>
+      <c r="I84" s="32" t="n">
+        <v>59.30615663528442</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Microbubble Air Circulator</t>
+          <t>Restored Harvester</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>68619</v>
+        <v>89206</v>
       </c>
       <c r="C85" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D85" s="19" t="n">
-        <v>179.9986267089844</v>
+        <v>0.9882170434577988</v>
+      </c>
+      <c r="D85" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E85" s="9" t="n">
+        <v>33.284792304039</v>
+      </c>
+      <c r="F85" s="9" t="n">
+        <v>109.9914312362671</v>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v/>
+      </c>
+      <c r="H85" s="9" t="n">
+        <v/>
+      </c>
+      <c r="I85" s="9" t="n">
+        <v>59.63026285171509</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="17" t="inlineStr">
-        <is>
-          <t>Microbubble Air Circulator</t>
-        </is>
-      </c>
-      <c r="B86" s="17" t="n">
-        <v>79741</v>
-      </c>
-      <c r="C86" s="18" t="n">
-        <v>0.9999990844475098</v>
-      </c>
-      <c r="D86" s="20" t="n">
-        <v>179.9985809326172</v>
-      </c>
-      <c r="E86" s="17" t="n"/>
-      <c r="F86" s="17" t="n"/>
-      <c r="G86" s="17" t="n"/>
-      <c r="H86" s="17" t="n"/>
-      <c r="I86" s="17" t="n"/>
+      <c r="A86" s="30" t="inlineStr">
+        <is>
+          <t>Reassembled Bulwark</t>
+        </is>
+      </c>
+      <c r="B86" s="30" t="n">
+        <v>39687</v>
+      </c>
+      <c r="C86" s="31" t="n">
+        <v>0.9881865577236336</v>
+      </c>
+      <c r="D86" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E86" s="32" t="n">
+        <v>34.07850861549377</v>
+      </c>
+      <c r="F86" s="32" t="n">
+        <v>109.3457102775574</v>
+      </c>
+      <c r="G86" s="32" t="n">
+        <v/>
+      </c>
+      <c r="H86" s="32" t="n">
+        <v/>
+      </c>
+      <c r="I86" s="32" t="n">
+        <v>59.45457220077515</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>Rebuilt Refractor</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>3850</v>
+      </c>
+      <c r="C87" s="8" t="n">
+        <v>0.9881172850151203</v>
+      </c>
+      <c r="D87" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E87" s="9" t="n">
+        <v>34.93671119213104</v>
+      </c>
+      <c r="F87" s="9" t="n">
+        <v/>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>73.53947162628174</v>
+      </c>
+      <c r="H87" s="9" t="n">
+        <v/>
+      </c>
+      <c r="I87" s="9" t="n">
+        <v>59.73169803619385</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="30" t="inlineStr">
+        <is>
+          <t>Improvised Oscillator</t>
+        </is>
+      </c>
+      <c r="B88" s="30" t="n">
+        <v>3153</v>
+      </c>
+      <c r="C88" s="31" t="n">
+        <v>0.9879791020175661</v>
+      </c>
+      <c r="D88" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E88" s="32" t="n">
+        <v>33.85613560676575</v>
+      </c>
+      <c r="F88" s="32" t="n">
+        <v>109.0752482414246</v>
+      </c>
+      <c r="G88" s="32" t="n">
+        <v/>
+      </c>
+      <c r="H88" s="32" t="n">
+        <v/>
+      </c>
+      <c r="I88" s="32" t="n">
+        <v>59.91156697273254</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Rusted Dampener</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>87108</v>
+      </c>
+      <c r="C89" s="8" t="n">
+        <v>0.9873884399115102</v>
+      </c>
+      <c r="D89" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E89" s="9" t="n">
+        <v>34.80534553527832</v>
+      </c>
+      <c r="F89" s="9" t="n">
+        <v>108.0902934074402</v>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v/>
+      </c>
+      <c r="H89" s="9" t="n">
+        <v/>
+      </c>
+      <c r="I89" s="9" t="n">
+        <v>59.81203317642212</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="30" t="inlineStr">
+        <is>
+          <t>Improvised Battery</t>
+        </is>
+      </c>
+      <c r="B90" s="30" t="n">
+        <v>53181</v>
+      </c>
+      <c r="C90" s="31" t="n">
+        <v>0.9872193519471507</v>
+      </c>
+      <c r="D90" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E90" s="32" t="n">
+        <v>33.65603983402252</v>
+      </c>
+      <c r="F90" s="32" t="n">
+        <v>109.8982691764832</v>
+      </c>
+      <c r="G90" s="32" t="n">
+        <v>73.85492324829102</v>
+      </c>
+      <c r="H90" s="32" t="n">
+        <v/>
+      </c>
+      <c r="I90" s="32" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Reassembled Stabiliser</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>69716</v>
+      </c>
+      <c r="C91" s="8" t="n">
+        <v>0.9863774662172949</v>
+      </c>
+      <c r="D91" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E91" s="9" t="n">
+        <v>34.77222919464111</v>
+      </c>
+      <c r="F91" s="9" t="n">
+        <v>109.6012234687805</v>
+      </c>
+      <c r="G91" s="9" t="n">
+        <v/>
+      </c>
+      <c r="H91" s="9" t="n">
+        <v/>
+      </c>
+      <c r="I91" s="9" t="n">
+        <v>58.16801786422729</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="30" t="inlineStr">
+        <is>
+          <t>Repaired Turbine</t>
+        </is>
+      </c>
+      <c r="B92" s="30" t="n">
+        <v>71097</v>
+      </c>
+      <c r="C92" s="31" t="n">
+        <v>0.9512280592485843</v>
+      </c>
+      <c r="D92" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E92" s="32" t="n">
+        <v>34.72938537597656</v>
+      </c>
+      <c r="F92" s="32" t="n">
+        <v/>
+      </c>
+      <c r="G92" s="32" t="n">
+        <v>70.04809379577637</v>
+      </c>
+      <c r="H92" s="32" t="n">
+        <v>29.09106612205505</v>
+      </c>
+      <c r="I92" s="32" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Adapted Refractor</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>76675</v>
+      </c>
+      <c r="C93" s="8" t="n">
+        <v>0.9406609089936614</v>
+      </c>
+      <c r="D93" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E93" s="9" t="n">
+        <v>32.00356960296631</v>
+      </c>
+      <c r="F93" s="29" t="n">
+        <v>109.9987745285034</v>
+      </c>
+      <c r="G93" s="9" t="n">
+        <v>65.89559316635132</v>
+      </c>
+      <c r="H93" s="9" t="n">
+        <v/>
+      </c>
+      <c r="I93" s="9" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="30" t="inlineStr">
+        <is>
+          <t>Adapted Dynamo</t>
+        </is>
+      </c>
+      <c r="B94" s="30" t="n">
+        <v>94592</v>
+      </c>
+      <c r="C94" s="31" t="n">
+        <v>0.9105828964836518</v>
+      </c>
+      <c r="D94" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E94" s="32" t="n">
+        <v>32.06693828105927</v>
+      </c>
+      <c r="F94" s="32" t="n">
+        <v>94.59738731384277</v>
+      </c>
+      <c r="G94" s="29" t="n">
+        <v>74.99861717224121</v>
+      </c>
+      <c r="H94" s="32" t="n">
+        <v/>
+      </c>
+      <c r="I94" s="32" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Rescued Amplifier</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>98822</v>
+      </c>
+      <c r="C95" s="8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D95" s="29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E95" s="29" t="n">
+        <v>34.99999940395355</v>
+      </c>
+      <c r="F95" s="9" t="n">
+        <v/>
+      </c>
+      <c r="G95" s="9" t="n">
+        <v/>
+      </c>
+      <c r="H95" s="9" t="n">
+        <v/>
+      </c>
+      <c r="I95" s="9" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="30" t="inlineStr">
+        <is>
+          <t>Recycled Accelerator</t>
+        </is>
+      </c>
+      <c r="B96" s="30" t="n">
+        <v>3260</v>
+      </c>
+      <c r="C96" s="31" t="n">
+        <v>0.383407556673834</v>
+      </c>
+      <c r="D96" s="32" t="n">
+        <v/>
+      </c>
+      <c r="E96" s="32" t="n">
+        <v>33.38805139064789</v>
+      </c>
+      <c r="F96" s="32" t="n">
+        <v/>
+      </c>
+      <c r="G96" s="32" t="n">
+        <v>3.348445892333984</v>
+      </c>
+      <c r="H96" s="32" t="n">
+        <v/>
+      </c>
+      <c r="I96" s="29" t="n">
+        <v>59.999680519104</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="21" t="inlineStr">
+        <is>
+          <t>Harmonic Splitter</t>
+        </is>
+      </c>
+      <c r="B97" s="21" t="n">
+        <v>43939</v>
+      </c>
+      <c r="C97" s="22" t="n">
+        <v>0.2321820391047452</v>
+      </c>
+      <c r="D97" s="23" t="n">
+        <v/>
+      </c>
+      <c r="E97" s="23" t="n">
+        <v/>
+      </c>
+      <c r="F97" s="23" t="n">
+        <v>39.96328711509705</v>
+      </c>
+      <c r="G97" s="23" t="n">
+        <v/>
+      </c>
+      <c r="H97" s="33" t="n">
+        <v>29.99853491783142</v>
+      </c>
+      <c r="I97" s="23" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="C98" s="4" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Aeration Membrane (UP_UNW)</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Seed</t>
+        </is>
+      </c>
+      <c r="C99" s="4" t="inlineStr">
+        <is>
+          <t>Perfection</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Oxygen Tank</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="14" t="inlineStr">
+        <is>
+          <t>Supreme Upgrade (3)</t>
+        </is>
+      </c>
+      <c r="B100" s="14" t="inlineStr"/>
+      <c r="C100" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" s="34" t="inlineStr">
+        <is>
+          <t>This technology is outdated in game version 4.40 as it was changed in 5.50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Microbubble Air Circulator</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>68619</v>
+      </c>
+      <c r="C101" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" s="19" t="n">
+        <v>179.9986267089844</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="17" t="inlineStr">
+        <is>
+          <t>Microbubble Air Circulator</t>
+        </is>
+      </c>
+      <c r="B102" s="17" t="n">
+        <v>79741</v>
+      </c>
+      <c r="C102" s="18" t="n">
+        <v>0.9999990844475098</v>
+      </c>
+      <c r="D102" s="20" t="n">
+        <v>179.9985809326172</v>
+      </c>
+      <c r="E102" s="17" t="n"/>
+      <c r="F102" s="17" t="n"/>
+      <c r="G102" s="17" t="n"/>
+      <c r="H102" s="17" t="n"/>
+      <c r="I102" s="17" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
           <t>Pure Oxygen Lung Replacement</t>
         </is>
       </c>
-      <c r="B87" t="n">
+      <c r="B103" t="n">
         <v>18072</v>
       </c>
-      <c r="C87" s="8" t="n">
+      <c r="C103" s="8" t="n">
         <v>0.9999984740791831</v>
       </c>
-      <c r="D87" s="9" t="n">
+      <c r="D103" s="9" t="n">
         <v>179.9985504150391</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="38" t="inlineStr">
+    <row r="104">
+      <c r="A104" s="35" t="inlineStr">
         <is>
           <t>Pure Oxygen Gas Pressurizer</t>
         </is>
       </c>
-      <c r="B88" s="38" t="n">
+      <c r="B104" s="35" t="n">
         <v>53523</v>
       </c>
-      <c r="C88" s="39" t="n">
+      <c r="C104" s="36" t="n">
         <v>0.9999493394288783</v>
       </c>
-      <c r="D88" s="40" t="n">
+      <c r="D104" s="37" t="n">
         <v>179.99609375</v>
       </c>
-      <c r="E88" s="38" t="n"/>
-      <c r="F88" s="38" t="n"/>
-      <c r="G88" s="38" t="n"/>
-      <c r="H88" s="38" t="n"/>
-      <c r="I88" s="38" t="n"/>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr"/>
-      <c r="C89" s="4" t="n"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="inlineStr">
-        <is>
-          <t>Radiation Protection (UP_RAD)</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Seed</t>
-        </is>
-      </c>
-      <c r="C90" s="4" t="inlineStr">
-        <is>
-          <t>Perfection</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Radiation Damage Shielding</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Radiation Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="14" t="inlineStr">
-        <is>
-          <t>Supreme Upgrade (3)</t>
-        </is>
-      </c>
-      <c r="B91" s="14" t="inlineStr"/>
-      <c r="C91" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D91" s="16" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Graded-Z DNA Repair System</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
-        <v>81124</v>
-      </c>
-      <c r="C92" s="8" t="n">
-        <v>0.9961528886530218</v>
-      </c>
-      <c r="D92" s="9" t="n">
-        <v>19.72635984420776</v>
-      </c>
-      <c r="E92" s="9" t="n">
-        <v>359.9459838867188</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="17" t="inlineStr">
-        <is>
-          <t>Electromagnetic Neutron Sink</t>
-        </is>
-      </c>
-      <c r="B93" s="17" t="n">
-        <v>51119</v>
-      </c>
-      <c r="C93" s="18" t="n">
-        <v>0.9944779888470059</v>
-      </c>
-      <c r="D93" s="20" t="n">
-        <v>19.950270652771</v>
-      </c>
-      <c r="E93" s="20" t="n">
-        <v>359.550537109375</v>
-      </c>
-      <c r="F93" s="17" t="n"/>
-      <c r="G93" s="17" t="n"/>
-      <c r="H93" s="17" t="n"/>
-      <c r="I93" s="17" t="n"/>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>Non-Linear Alpha Barrier</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>47825</v>
-      </c>
-      <c r="C94" s="8" t="n">
-        <v>0.9935507326500348</v>
-      </c>
-      <c r="D94" s="9" t="n">
-        <v>19.9059784412384</v>
-      </c>
-      <c r="E94" s="9" t="n">
-        <v>359.514404296875</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="17" t="inlineStr">
-        <is>
-          <t>Non-Linear Ion Shield</t>
-        </is>
-      </c>
-      <c r="B95" s="17" t="n">
-        <v>31472</v>
-      </c>
-      <c r="C95" s="18" t="n">
-        <v>0.9197621136413663</v>
-      </c>
-      <c r="D95" s="20" t="n">
-        <v>13.2892370223999</v>
-      </c>
-      <c r="E95" s="19" t="n">
-        <v>359.9983520507812</v>
-      </c>
-      <c r="F95" s="17" t="n"/>
-      <c r="G95" s="17" t="n"/>
-      <c r="H95" s="17" t="n"/>
-      <c r="I95" s="17" t="n"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="21" t="inlineStr">
-        <is>
-          <t>Quantum Bio-Integrity Unit</t>
-        </is>
-      </c>
-      <c r="B96" s="21" t="n">
-        <v>66946</v>
-      </c>
-      <c r="C96" s="22" t="n">
-        <v>0.1323911635222846</v>
-      </c>
-      <c r="D96" s="24" t="n">
-        <v>19.99990940093994</v>
-      </c>
-      <c r="E96" s="23" t="n">
-        <v>281.165283203125</v>
-      </c>
-      <c r="F96" s="21" t="n"/>
-      <c r="G96" s="21" t="n"/>
-      <c r="H96" s="21" t="n"/>
-      <c r="I96" s="21" t="n"/>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr"/>
-      <c r="C97" s="4" t="n"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>Toxic Protection (UP_TOX)</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Seed</t>
-        </is>
-      </c>
-      <c r="C98" s="4" t="inlineStr">
-        <is>
-          <t>Perfection</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Toxic Damage Shielding</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Toxic Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="14" t="inlineStr">
-        <is>
-          <t>Supreme Upgrade (3)</t>
-        </is>
-      </c>
-      <c r="B99" s="14" t="inlineStr"/>
-      <c r="C99" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D99" s="16" t="inlineStr"/>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>Gigawatt De-toxifier</t>
-        </is>
-      </c>
-      <c r="B100" t="n">
-        <v>81124</v>
-      </c>
-      <c r="C100" s="8" t="n">
-        <v>0.9961528886530218</v>
-      </c>
-      <c r="D100" s="9" t="n">
-        <v>19.72635984420776</v>
-      </c>
-      <c r="E100" s="9" t="n">
-        <v>359.9459838867188</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="17" t="inlineStr">
-        <is>
-          <t>Irradiating Biohazard Filter</t>
-        </is>
-      </c>
-      <c r="B101" s="17" t="n">
-        <v>51119</v>
-      </c>
-      <c r="C101" s="18" t="n">
-        <v>0.9944779888470059</v>
-      </c>
-      <c r="D101" s="20" t="n">
-        <v>19.950270652771</v>
-      </c>
-      <c r="E101" s="20" t="n">
-        <v>359.550537109375</v>
-      </c>
-      <c r="F101" s="17" t="n"/>
-      <c r="G101" s="17" t="n"/>
-      <c r="H101" s="17" t="n"/>
-      <c r="I101" s="17" t="n"/>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>Vermiform Microfilters</t>
-        </is>
-      </c>
-      <c r="B102" t="n">
-        <v>47825</v>
-      </c>
-      <c r="C102" s="8" t="n">
-        <v>0.9935507326500348</v>
-      </c>
-      <c r="D102" s="9" t="n">
-        <v>19.9059784412384</v>
-      </c>
-      <c r="E102" s="9" t="n">
-        <v>359.514404296875</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="17" t="inlineStr">
-        <is>
-          <t>Vermiform Exhaust Filter</t>
-        </is>
-      </c>
-      <c r="B103" s="17" t="n">
-        <v>31472</v>
-      </c>
-      <c r="C103" s="18" t="n">
-        <v>0.9197621136413663</v>
-      </c>
-      <c r="D103" s="20" t="n">
-        <v>13.2892370223999</v>
-      </c>
-      <c r="E103" s="19" t="n">
-        <v>359.9983520507812</v>
-      </c>
-      <c r="F103" s="17" t="n"/>
-      <c r="G103" s="17" t="n"/>
-      <c r="H103" s="17" t="n"/>
-      <c r="I103" s="17" t="n"/>
-    </row>
-    <row r="104">
-      <c r="A104" s="21" t="inlineStr">
-        <is>
-          <t>Vacuum Gas Scrubber</t>
-        </is>
-      </c>
-      <c r="B104" s="21" t="n">
-        <v>66946</v>
-      </c>
-      <c r="C104" s="22" t="n">
-        <v>0.1323911635222846</v>
-      </c>
-      <c r="D104" s="24" t="n">
-        <v>19.99990940093994</v>
-      </c>
-      <c r="E104" s="23" t="n">
-        <v>281.165283203125</v>
-      </c>
-      <c r="F104" s="21" t="n"/>
-      <c r="G104" s="21" t="n"/>
-      <c r="H104" s="21" t="n"/>
-      <c r="I104" s="21" t="n"/>
+      <c r="E104" s="35" t="n"/>
+      <c r="F104" s="35" t="n"/>
+      <c r="G104" s="35" t="n"/>
+      <c r="H104" s="35" t="n"/>
+      <c r="I104" s="35" t="n"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr"/>
@@ -4160,7 +4357,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>Cold Protection (UP_COLD)</t>
+          <t>Radiation Protection (UP_RAD)</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -4175,12 +4372,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Cold Damage Shielding</t>
+          <t>Radiation Damage Shielding</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Cold Protection</t>
+          <t>Radiation Protection</t>
         </is>
       </c>
     </row>
@@ -4199,7 +4396,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Unfreezable Radiator Unit</t>
+          <t>Graded-Z DNA Repair System</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -4218,7 +4415,7 @@
     <row r="109">
       <c r="A109" s="17" t="inlineStr">
         <is>
-          <t>Cryostatic Boiler System</t>
+          <t>Electromagnetic Neutron Sink</t>
         </is>
       </c>
       <c r="B109" s="17" t="n">
@@ -4241,7 +4438,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Solvent-Fueled Ice Shield</t>
+          <t>Non-Linear Alpha Barrier</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -4260,7 +4457,7 @@
     <row r="111">
       <c r="A111" s="17" t="inlineStr">
         <is>
-          <t>Solvent-Fueled Thermal Harvester</t>
+          <t>Non-Linear Ion Shield</t>
         </is>
       </c>
       <c r="B111" s="17" t="n">
@@ -4283,7 +4480,7 @@
     <row r="112">
       <c r="A112" s="21" t="inlineStr">
         <is>
-          <t>Energy Field Insulation</t>
+          <t>Quantum Bio-Integrity Unit</t>
         </is>
       </c>
       <c r="B112" s="21" t="n">
@@ -4310,7 +4507,7 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>Heat Protection (UP_HOT)</t>
+          <t>Toxic Protection (UP_TOX)</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -4325,12 +4522,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Heat Damage Shielding</t>
+          <t>Toxic Damage Shielding</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Heat Protection</t>
+          <t>Toxic Protection</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4546,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Infrared Thermal Barrier</t>
+          <t>Gigawatt De-toxifier</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -4368,7 +4565,7 @@
     <row r="117">
       <c r="A117" s="17" t="inlineStr">
         <is>
-          <t>Negative Energy Heliostat</t>
+          <t>Irradiating Biohazard Filter</t>
         </is>
       </c>
       <c r="B117" s="17" t="n">
@@ -4391,7 +4588,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Ablative Infrared Deflector</t>
+          <t>Vermiform Microfilters</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -4410,7 +4607,7 @@
     <row r="119">
       <c r="A119" s="17" t="inlineStr">
         <is>
-          <t>Ablative Atmosphere Regulator</t>
+          <t>Vermiform Exhaust Filter</t>
         </is>
       </c>
       <c r="B119" s="17" t="n">
@@ -4433,7 +4630,7 @@
     <row r="120">
       <c r="A120" s="21" t="inlineStr">
         <is>
-          <t>Carbon-Bonded Thermoregulator</t>
+          <t>Vacuum Gas Scrubber</t>
         </is>
       </c>
       <c r="B120" s="21" t="n">
@@ -4455,23 +4652,323 @@
     </row>
     <row r="121">
       <c r="A121" t="inlineStr"/>
+      <c r="C121" s="4" t="n"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>Cold Protection (UP_COLD)</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Seed</t>
+        </is>
+      </c>
+      <c r="C122" s="4" t="inlineStr">
+        <is>
+          <t>Perfection</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Cold Damage Shielding</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Cold Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="14" t="inlineStr">
+        <is>
+          <t>Supreme Upgrade (3)</t>
+        </is>
+      </c>
+      <c r="B123" s="14" t="inlineStr"/>
+      <c r="C123" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D123" s="16" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Unfreezable Radiator Unit</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>81124</v>
+      </c>
+      <c r="C124" s="8" t="n">
+        <v>0.9961528886530218</v>
+      </c>
+      <c r="D124" s="9" t="n">
+        <v>19.72635984420776</v>
+      </c>
+      <c r="E124" s="9" t="n">
+        <v>359.9459838867188</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="17" t="inlineStr">
+        <is>
+          <t>Cryostatic Boiler System</t>
+        </is>
+      </c>
+      <c r="B125" s="17" t="n">
+        <v>51119</v>
+      </c>
+      <c r="C125" s="18" t="n">
+        <v>0.9944779888470059</v>
+      </c>
+      <c r="D125" s="20" t="n">
+        <v>19.950270652771</v>
+      </c>
+      <c r="E125" s="20" t="n">
+        <v>359.550537109375</v>
+      </c>
+      <c r="F125" s="17" t="n"/>
+      <c r="G125" s="17" t="n"/>
+      <c r="H125" s="17" t="n"/>
+      <c r="I125" s="17" t="n"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Solvent-Fueled Ice Shield</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>47825</v>
+      </c>
+      <c r="C126" s="8" t="n">
+        <v>0.9935507326500348</v>
+      </c>
+      <c r="D126" s="9" t="n">
+        <v>19.9059784412384</v>
+      </c>
+      <c r="E126" s="9" t="n">
+        <v>359.514404296875</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="17" t="inlineStr">
+        <is>
+          <t>Solvent-Fueled Thermal Harvester</t>
+        </is>
+      </c>
+      <c r="B127" s="17" t="n">
+        <v>31472</v>
+      </c>
+      <c r="C127" s="18" t="n">
+        <v>0.9197621136413663</v>
+      </c>
+      <c r="D127" s="20" t="n">
+        <v>13.2892370223999</v>
+      </c>
+      <c r="E127" s="19" t="n">
+        <v>359.9983520507812</v>
+      </c>
+      <c r="F127" s="17" t="n"/>
+      <c r="G127" s="17" t="n"/>
+      <c r="H127" s="17" t="n"/>
+      <c r="I127" s="17" t="n"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="21" t="inlineStr">
+        <is>
+          <t>Energy Field Insulation</t>
+        </is>
+      </c>
+      <c r="B128" s="21" t="n">
+        <v>66946</v>
+      </c>
+      <c r="C128" s="22" t="n">
+        <v>0.1323911635222846</v>
+      </c>
+      <c r="D128" s="24" t="n">
+        <v>19.99990940093994</v>
+      </c>
+      <c r="E128" s="23" t="n">
+        <v>281.165283203125</v>
+      </c>
+      <c r="F128" s="21" t="n"/>
+      <c r="G128" s="21" t="n"/>
+      <c r="H128" s="21" t="n"/>
+      <c r="I128" s="21" t="n"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="C129" s="4" t="n"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>Heat Protection (UP_HOT)</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Seed</t>
+        </is>
+      </c>
+      <c r="C130" s="4" t="inlineStr">
+        <is>
+          <t>Perfection</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Heat Damage Shielding</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Heat Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="14" t="inlineStr">
+        <is>
+          <t>Supreme Upgrade (3)</t>
+        </is>
+      </c>
+      <c r="B131" s="14" t="inlineStr"/>
+      <c r="C131" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D131" s="16" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Infrared Thermal Barrier</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>81124</v>
+      </c>
+      <c r="C132" s="8" t="n">
+        <v>0.9961528886530218</v>
+      </c>
+      <c r="D132" s="9" t="n">
+        <v>19.72635984420776</v>
+      </c>
+      <c r="E132" s="9" t="n">
+        <v>359.9459838867188</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="17" t="inlineStr">
+        <is>
+          <t>Negative Energy Heliostat</t>
+        </is>
+      </c>
+      <c r="B133" s="17" t="n">
+        <v>51119</v>
+      </c>
+      <c r="C133" s="18" t="n">
+        <v>0.9944779888470059</v>
+      </c>
+      <c r="D133" s="20" t="n">
+        <v>19.950270652771</v>
+      </c>
+      <c r="E133" s="20" t="n">
+        <v>359.550537109375</v>
+      </c>
+      <c r="F133" s="17" t="n"/>
+      <c r="G133" s="17" t="n"/>
+      <c r="H133" s="17" t="n"/>
+      <c r="I133" s="17" t="n"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Ablative Infrared Deflector</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>47825</v>
+      </c>
+      <c r="C134" s="8" t="n">
+        <v>0.9935507326500348</v>
+      </c>
+      <c r="D134" s="9" t="n">
+        <v>19.9059784412384</v>
+      </c>
+      <c r="E134" s="9" t="n">
+        <v>359.514404296875</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="17" t="inlineStr">
+        <is>
+          <t>Ablative Atmosphere Regulator</t>
+        </is>
+      </c>
+      <c r="B135" s="17" t="n">
+        <v>31472</v>
+      </c>
+      <c r="C135" s="18" t="n">
+        <v>0.9197621136413663</v>
+      </c>
+      <c r="D135" s="20" t="n">
+        <v>13.2892370223999</v>
+      </c>
+      <c r="E135" s="19" t="n">
+        <v>359.9983520507812</v>
+      </c>
+      <c r="F135" s="17" t="n"/>
+      <c r="G135" s="17" t="n"/>
+      <c r="H135" s="17" t="n"/>
+      <c r="I135" s="17" t="n"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="21" t="inlineStr">
+        <is>
+          <t>Carbon-Bonded Thermoregulator</t>
+        </is>
+      </c>
+      <c r="B136" s="21" t="n">
+        <v>66946</v>
+      </c>
+      <c r="C136" s="22" t="n">
+        <v>0.1323911635222846</v>
+      </c>
+      <c r="D136" s="24" t="n">
+        <v>19.99990940093994</v>
+      </c>
+      <c r="E136" s="23" t="n">
+        <v>281.165283203125</v>
+      </c>
+      <c r="F136" s="21" t="n"/>
+      <c r="G136" s="21" t="n"/>
+      <c r="H136" s="21" t="n"/>
+      <c r="I136" s="21" t="n"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="D24:I24"/>
     <mergeCell ref="D2:I2"/>
-    <mergeCell ref="D81:I81"/>
-    <mergeCell ref="D99:I99"/>
+    <mergeCell ref="D100:I100"/>
     <mergeCell ref="D14:I14"/>
-    <mergeCell ref="D84:I84"/>
     <mergeCell ref="D107:I107"/>
+    <mergeCell ref="D123:I123"/>
     <mergeCell ref="D40:I40"/>
+    <mergeCell ref="D131:I131"/>
     <mergeCell ref="D58:I58"/>
-    <mergeCell ref="D91:I91"/>
     <mergeCell ref="D115:I115"/>
     <mergeCell ref="D52:I52"/>
     <mergeCell ref="D8:I8"/>
     <mergeCell ref="D64:I64"/>
+    <mergeCell ref="D82:I82"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5741,18 +6238,18 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="38" t="inlineStr">
+      <c r="A62" s="35" t="inlineStr">
         <is>
           <t>Free Electron Refractor</t>
         </is>
       </c>
-      <c r="B62" s="38" t="n">
+      <c r="B62" s="35" t="n">
         <v>91149</v>
       </c>
-      <c r="C62" s="39" t="n">
+      <c r="C62" s="36" t="n">
         <v>0.9999765915040814</v>
       </c>
-      <c r="D62" s="40" t="n">
+      <c r="D62" s="37" t="n">
         <v>27.99971961975098</v>
       </c>
       <c r="E62" s="24" t="n">
@@ -5761,9 +6258,9 @@
       <c r="F62" s="24" t="n">
         <v>2.100002765655518</v>
       </c>
-      <c r="G62" s="38" t="n"/>
-      <c r="H62" s="38" t="n"/>
-      <c r="I62" s="38" t="n"/>
+      <c r="G62" s="35" t="n"/>
+      <c r="H62" s="35" t="n"/>
+      <c r="I62" s="35" t="n"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
@@ -6259,29 +6756,29 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="38" t="inlineStr">
+      <c r="A88" s="35" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B88" s="38" t="n">
+      <c r="B88" s="35" t="n">
         <v>3014</v>
       </c>
-      <c r="C88" s="39" t="n">
+      <c r="C88" s="36" t="n">
         <v>0.2393532220868545</v>
       </c>
       <c r="D88" s="24" t="n">
         <v>7.999974250793457</v>
       </c>
-      <c r="E88" s="40" t="n">
+      <c r="E88" s="37" t="n">
         <v>6.08595609664917</v>
       </c>
-      <c r="F88" s="40" t="n">
+      <c r="F88" s="37" t="n">
         <v>6.003260612487793</v>
       </c>
-      <c r="G88" s="38" t="n"/>
-      <c r="H88" s="38" t="n"/>
-      <c r="I88" s="38" t="n"/>
+      <c r="G88" s="35" t="n"/>
+      <c r="H88" s="35" t="n"/>
+      <c r="I88" s="35" t="n"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -6554,29 +7051,29 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="38" t="inlineStr">
+      <c r="A102" s="35" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B102" s="38" t="n">
+      <c r="B102" s="35" t="n">
         <v>3014</v>
       </c>
-      <c r="C102" s="39" t="n">
+      <c r="C102" s="36" t="n">
         <v>0.3009311425696053</v>
       </c>
       <c r="D102" s="24" t="n">
         <v>11.99998664855957</v>
       </c>
-      <c r="E102" s="40" t="n">
+      <c r="E102" s="37" t="n">
         <v>7.293200492858887</v>
       </c>
-      <c r="F102" s="40" t="n">
+      <c r="F102" s="37" t="n">
         <v>5.142772197723389</v>
       </c>
-      <c r="G102" s="38" t="n"/>
-      <c r="H102" s="38" t="n"/>
-      <c r="I102" s="38" t="n"/>
+      <c r="G102" s="35" t="n"/>
+      <c r="H102" s="35" t="n"/>
+      <c r="I102" s="35" t="n"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr"/>
@@ -6849,29 +7346,29 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="38" t="inlineStr">
+      <c r="A116" s="35" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B116" s="38" t="n">
+      <c r="B116" s="35" t="n">
         <v>3014</v>
       </c>
-      <c r="C116" s="39" t="n">
+      <c r="C116" s="36" t="n">
         <v>0.2700637885284971</v>
       </c>
       <c r="D116" s="24" t="n">
         <v>11.99998664855957</v>
       </c>
-      <c r="E116" s="40" t="n">
+      <c r="E116" s="37" t="n">
         <v>30.73297739028931</v>
       </c>
-      <c r="F116" s="40" t="n">
+      <c r="F116" s="37" t="n">
         <v>10.14277935028076</v>
       </c>
-      <c r="G116" s="38" t="n"/>
-      <c r="H116" s="38" t="n"/>
-      <c r="I116" s="38" t="n"/>
+      <c r="G116" s="35" t="n"/>
+      <c r="H116" s="35" t="n"/>
+      <c r="I116" s="35" t="n"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr"/>
@@ -7606,18 +8103,18 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="38" t="inlineStr">
+      <c r="A34" s="35" t="inlineStr">
         <is>
           <t>Boundless Gills</t>
         </is>
       </c>
-      <c r="B34" s="38" t="n">
+      <c r="B34" s="35" t="n">
         <v>95566</v>
       </c>
-      <c r="C34" s="39" t="n">
+      <c r="C34" s="36" t="n">
         <v>0.9999561090701528</v>
       </c>
-      <c r="D34" s="40" t="n">
+      <c r="D34" s="37" t="n">
         <v>27.99951934814453</v>
       </c>
       <c r="E34" s="24" t="n">
@@ -7626,9 +8123,9 @@
       <c r="F34" s="24" t="n">
         <v>2.100002765655518</v>
       </c>
-      <c r="G34" s="38" t="n"/>
-      <c r="H34" s="38" t="n"/>
-      <c r="I34" s="38" t="n"/>
+      <c r="G34" s="35" t="n"/>
+      <c r="H34" s="35" t="n"/>
+      <c r="I34" s="35" t="n"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -7936,29 +8433,29 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="38" t="inlineStr">
+      <c r="A49" s="35" t="inlineStr">
         <is>
           <t>Vibrant Fluids</t>
         </is>
       </c>
-      <c r="B49" s="38" t="n">
+      <c r="B49" s="35" t="n">
         <v>96019</v>
       </c>
-      <c r="C49" s="39" t="n">
+      <c r="C49" s="36" t="n">
         <v>0.07136355988009535</v>
       </c>
-      <c r="D49" s="40" t="n">
-        <v/>
-      </c>
-      <c r="E49" s="40" t="n">
+      <c r="D49" s="37" t="n">
+        <v/>
+      </c>
+      <c r="E49" s="37" t="n">
         <v>75.4543662071228</v>
       </c>
       <c r="F49" s="24" t="n">
         <v>0.299999475479126</v>
       </c>
-      <c r="G49" s="38" t="n"/>
-      <c r="H49" s="38" t="n"/>
-      <c r="I49" s="38" t="n"/>
+      <c r="G49" s="35" t="n"/>
+      <c r="H49" s="35" t="n"/>
+      <c r="I49" s="35" t="n"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -10154,16 +10651,16 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="41" t="inlineStr">
+      <c r="A84" s="38" t="inlineStr">
         <is>
           <t>Upgrade (1)</t>
         </is>
       </c>
-      <c r="B84" s="41" t="inlineStr"/>
-      <c r="C84" s="42" t="n">
+      <c r="B84" s="38" t="inlineStr"/>
+      <c r="C84" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="D84" s="43" t="inlineStr"/>
+      <c r="D84" s="40" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -10177,7 +10674,7 @@
       <c r="C85" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D85" s="44" t="n">
+      <c r="D85" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E85" s="9" t="n">
@@ -10186,36 +10683,36 @@
       <c r="F85" s="9" t="n">
         <v/>
       </c>
-      <c r="G85" s="44" t="n">
+      <c r="G85" s="41" t="n">
         <v>199.9960780143738</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="45" t="inlineStr">
+      <c r="A86" s="42" t="inlineStr">
         <is>
           <t>Tertiary Injector Plugs</t>
         </is>
       </c>
-      <c r="B86" s="45" t="n">
+      <c r="B86" s="42" t="n">
         <v>66503</v>
       </c>
-      <c r="C86" s="46" t="n">
+      <c r="C86" s="43" t="n">
         <v>0.9638186662144554</v>
       </c>
-      <c r="D86" s="47" t="n">
-        <v/>
-      </c>
-      <c r="E86" s="47" t="n">
+      <c r="D86" s="44" t="n">
+        <v/>
+      </c>
+      <c r="E86" s="44" t="n">
         <v>196.2135009765625</v>
       </c>
-      <c r="F86" s="47" t="n">
-        <v/>
-      </c>
-      <c r="G86" s="47" t="n">
+      <c r="F86" s="44" t="n">
+        <v/>
+      </c>
+      <c r="G86" s="44" t="n">
         <v>196.5467929840088</v>
       </c>
-      <c r="H86" s="45" t="n"/>
-      <c r="I86" s="45" t="n"/>
+      <c r="H86" s="42" t="n"/>
+      <c r="I86" s="42" t="n"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -10243,31 +10740,31 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="45" t="inlineStr">
+      <c r="A88" s="42" t="inlineStr">
         <is>
           <t>Efficient Coils</t>
         </is>
       </c>
-      <c r="B88" s="45" t="n">
+      <c r="B88" s="42" t="n">
         <v>38522</v>
       </c>
-      <c r="C88" s="46" t="n">
+      <c r="C88" s="43" t="n">
         <v>0.9455232585792177</v>
       </c>
-      <c r="D88" s="47" t="n">
-        <v/>
-      </c>
-      <c r="E88" s="47" t="n">
+      <c r="D88" s="44" t="n">
+        <v/>
+      </c>
+      <c r="E88" s="44" t="n">
         <v>190.1379699707031</v>
       </c>
-      <c r="F88" s="47" t="n">
-        <v/>
-      </c>
-      <c r="G88" s="47" t="n">
+      <c r="F88" s="44" t="n">
+        <v/>
+      </c>
+      <c r="G88" s="44" t="n">
         <v>198.9651203155518</v>
       </c>
-      <c r="H88" s="45" t="n"/>
-      <c r="I88" s="45" t="n"/>
+      <c r="H88" s="42" t="n"/>
+      <c r="I88" s="42" t="n"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -10295,31 +10792,31 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="45" t="inlineStr">
+      <c r="A90" s="42" t="inlineStr">
         <is>
           <t>Lubricated Timing Loom</t>
         </is>
       </c>
-      <c r="B90" s="45" t="n">
+      <c r="B90" s="42" t="n">
         <v>81042</v>
       </c>
-      <c r="C90" s="46" t="n">
+      <c r="C90" s="43" t="n">
         <v>0.5</v>
       </c>
-      <c r="D90" s="47" t="n">
-        <v/>
-      </c>
-      <c r="E90" s="44" t="n">
+      <c r="D90" s="44" t="n">
+        <v/>
+      </c>
+      <c r="E90" s="41" t="n">
         <v>199.9966888427734</v>
       </c>
-      <c r="F90" s="47" t="n">
-        <v/>
-      </c>
-      <c r="G90" s="47" t="n">
-        <v/>
-      </c>
-      <c r="H90" s="45" t="n"/>
-      <c r="I90" s="45" t="n"/>
+      <c r="F90" s="44" t="n">
+        <v/>
+      </c>
+      <c r="G90" s="44" t="n">
+        <v/>
+      </c>
+      <c r="H90" s="42" t="n"/>
+      <c r="I90" s="42" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="21" t="inlineStr">
@@ -10339,7 +10836,7 @@
       <c r="E91" s="23" t="n">
         <v/>
       </c>
-      <c r="F91" s="48" t="n">
+      <c r="F91" s="45" t="n">
         <v>4.999732971191406</v>
       </c>
       <c r="G91" s="23" t="n">
@@ -10807,29 +11304,29 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="38" t="inlineStr">
+      <c r="A113" s="35" t="inlineStr">
         <is>
           <t>Nano-Boosted Core</t>
         </is>
       </c>
-      <c r="B113" s="38" t="n">
+      <c r="B113" s="35" t="n">
         <v>96019</v>
       </c>
-      <c r="C113" s="39" t="n">
+      <c r="C113" s="36" t="n">
         <v>0.6721026498583409</v>
       </c>
-      <c r="D113" s="40" t="n">
+      <c r="D113" s="37" t="n">
         <v>351.1358947753906</v>
       </c>
-      <c r="E113" s="40" t="n">
+      <c r="E113" s="37" t="n">
         <v/>
       </c>
       <c r="F113" s="24" t="n">
         <v>299.9994516372681</v>
       </c>
-      <c r="G113" s="38" t="n"/>
-      <c r="H113" s="38" t="n"/>
-      <c r="I113" s="38" t="n"/>
+      <c r="G113" s="35" t="n"/>
+      <c r="H113" s="35" t="n"/>
+      <c r="I113" s="35" t="n"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr"/>
@@ -12301,9 +12798,9 @@
       <c r="C172" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D172" s="37" t="inlineStr">
-        <is>
-          <t>This technology is outdated in game version 4.30 as it was changed in 5.50.</t>
+      <c r="D172" s="34" t="inlineStr">
+        <is>
+          <t>This technology is outdated in game version 4.40 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -12796,29 +13293,29 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="49" t="inlineStr">
+      <c r="A194" s="46" t="inlineStr">
         <is>
           <t>Forsaken Capacitor</t>
         </is>
       </c>
-      <c r="B194" s="49" t="n">
+      <c r="B194" s="46" t="n">
         <v>55029</v>
       </c>
-      <c r="C194" s="50" t="n">
+      <c r="C194" s="47" t="n">
         <v>0.5019393878517006</v>
       </c>
       <c r="D194" s="33" t="n">
         <v>3.999966144561768</v>
       </c>
-      <c r="E194" s="51" t="n">
-        <v/>
-      </c>
-      <c r="F194" s="51" t="n">
+      <c r="E194" s="48" t="n">
+        <v/>
+      </c>
+      <c r="F194" s="48" t="n">
         <v>10.61809062957764</v>
       </c>
-      <c r="G194" s="49" t="n"/>
-      <c r="H194" s="49" t="n"/>
-      <c r="I194" s="49" t="n"/>
+      <c r="G194" s="46" t="n"/>
+      <c r="H194" s="46" t="n"/>
+      <c r="I194" s="46" t="n"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr"/>
@@ -13036,29 +13533,29 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="38" t="inlineStr">
+      <c r="A8" s="35" t="inlineStr">
         <is>
           <t>Faultless Recycler</t>
         </is>
       </c>
-      <c r="B8" s="38" t="n">
+      <c r="B8" s="35" t="n">
         <v>32361</v>
       </c>
-      <c r="C8" s="39" t="n">
+      <c r="C8" s="36" t="n">
         <v>0.2099291858044448</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="37" t="n">
         <v>30.36361312866211</v>
       </c>
-      <c r="E8" s="40" t="n">
+      <c r="E8" s="37" t="n">
         <v>15.00709652900696</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>9.999978542327881</v>
       </c>
-      <c r="G8" s="38" t="n"/>
-      <c r="H8" s="38" t="n"/>
-      <c r="I8" s="38" t="n"/>
+      <c r="G8" s="35" t="n"/>
+      <c r="H8" s="35" t="n"/>
+      <c r="I8" s="35" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -13591,9 +14088,9 @@
       <c r="C2" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="inlineStr">
-        <is>
-          <t>This technology is outdated in game version 4.30 as it was changed in 5.50.</t>
+      <c r="D2" s="34" t="inlineStr">
+        <is>
+          <t>This technology is outdated in game version 4.40 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -13714,18 +14211,18 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="38" t="inlineStr">
+      <c r="A8" s="35" t="inlineStr">
         <is>
           <t>High Pressure Turbine Controller</t>
         </is>
       </c>
-      <c r="B8" s="38" t="n">
+      <c r="B8" s="35" t="n">
         <v>96019</v>
       </c>
-      <c r="C8" s="39" t="n">
+      <c r="C8" s="36" t="n">
         <v>0.8061205041219637</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="37" t="n">
         <v>25.81901550292969</v>
       </c>
       <c r="E8" s="24" t="n">
@@ -13734,9 +14231,9 @@
       <c r="F8" s="24" t="n">
         <v>29.99997437000275</v>
       </c>
-      <c r="G8" s="38" t="n"/>
-      <c r="H8" s="38" t="n"/>
-      <c r="I8" s="38" t="n"/>
+      <c r="G8" s="35" t="n"/>
+      <c r="H8" s="35" t="n"/>
+      <c r="I8" s="35" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -14236,29 +14733,29 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="38" t="inlineStr">
+      <c r="A16" s="35" t="inlineStr">
         <is>
           <t>Faultless Recycler</t>
         </is>
       </c>
-      <c r="B16" s="38" t="n">
+      <c r="B16" s="35" t="n">
         <v>32361</v>
       </c>
-      <c r="C16" s="39" t="n">
+      <c r="C16" s="36" t="n">
         <v>0.2099282888068533</v>
       </c>
-      <c r="D16" s="40" t="n">
+      <c r="D16" s="37" t="n">
         <v>30.36361312866211</v>
       </c>
-      <c r="E16" s="40" t="n">
+      <c r="E16" s="37" t="n">
         <v>15.00709652900696</v>
       </c>
       <c r="F16" s="24" t="n">
         <v>9.999954700469971</v>
       </c>
-      <c r="G16" s="38" t="n"/>
-      <c r="H16" s="38" t="n"/>
-      <c r="I16" s="38" t="n"/>
+      <c r="G16" s="35" t="n"/>
+      <c r="H16" s="35" t="n"/>
+      <c r="I16" s="35" t="n"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -14415,7 +14912,7 @@
       <c r="C25" s="4" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="34" t="inlineStr">
+      <c r="A26" s="49" t="inlineStr">
         <is>
           <t>Minotaur Flamethrower (UP_MFIRE)</t>
         </is>
@@ -14425,14 +14922,14 @@
           <t>Seed</t>
         </is>
       </c>
-      <c r="C26" s="35" t="inlineStr">
+      <c r="C26" s="50" t="inlineStr">
         <is>
           <t>Perfection</t>
         </is>
       </c>
-      <c r="D26" s="36" t="inlineStr">
-        <is>
-          <t>This technology is not yet available in game version 4.30 but was added in 5.00.</t>
+      <c r="D26" s="51" t="inlineStr">
+        <is>
+          <t>This technology is not yet available in game version 4.40 but was added in 5.00.</t>
         </is>
       </c>
       <c r="E26" s="21" t="n"/>
@@ -14781,25 +15278,25 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="38" t="inlineStr">
+      <c r="A18" s="35" t="inlineStr">
         <is>
           <t>Navigation AI Unit from SS Emperor Bayaseb</t>
         </is>
       </c>
-      <c r="B18" s="38" t="n">
+      <c r="B18" s="35" t="n">
         <v>88814</v>
       </c>
-      <c r="C18" s="39" t="n">
+      <c r="C18" s="36" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="24" t="n">
         <v>19.9999988079071</v>
       </c>
-      <c r="E18" s="38" t="n"/>
-      <c r="F18" s="38" t="n"/>
-      <c r="G18" s="38" t="n"/>
-      <c r="H18" s="38" t="n"/>
-      <c r="I18" s="38" t="n"/>
+      <c r="E18" s="35" t="n"/>
+      <c r="F18" s="35" t="n"/>
+      <c r="G18" s="35" t="n"/>
+      <c r="H18" s="35" t="n"/>
+      <c r="I18" s="35" t="n"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>

</xml_diff>

<commit_message>
chore(game): update to 5.00
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -200,11 +200,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -604,7 +599,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>4.40</t>
+          <t>5.00</t>
         </is>
       </c>
     </row>
@@ -1215,7 +1210,7 @@
       <c r="B3" t="n">
         <v>91860</v>
       </c>
-      <c r="C3" s="52" t="n">
+      <c r="C3" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
@@ -1246,7 +1241,7 @@
       <c r="B6" t="n">
         <v>91860</v>
       </c>
-      <c r="C6" s="52" t="n">
+      <c r="C6" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
@@ -1277,7 +1272,7 @@
       <c r="B9" t="n">
         <v>91860</v>
       </c>
-      <c r="C9" s="52" t="n">
+      <c r="C9" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
@@ -1308,7 +1303,7 @@
       <c r="B12" t="n">
         <v>91860</v>
       </c>
-      <c r="C12" s="52" t="n">
+      <c r="C12" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D12" t="n">
@@ -1339,7 +1334,7 @@
       <c r="B15" t="n">
         <v>91860</v>
       </c>
-      <c r="C15" s="52" t="n">
+      <c r="C15" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
@@ -1370,7 +1365,7 @@
       <c r="B18" t="n">
         <v>91860</v>
       </c>
-      <c r="C18" s="52" t="n">
+      <c r="C18" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D18" t="n">
@@ -1401,7 +1396,7 @@
       <c r="B21" t="n">
         <v>91860</v>
       </c>
-      <c r="C21" s="52" t="n">
+      <c r="C21" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D21" t="n">
@@ -1432,7 +1427,7 @@
       <c r="B24" t="n">
         <v>91860</v>
       </c>
-      <c r="C24" s="52" t="n">
+      <c r="C24" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
@@ -1463,7 +1458,7 @@
       <c r="B27" t="n">
         <v>91860</v>
       </c>
-      <c r="C27" s="52" t="n">
+      <c r="C27" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D27" t="n">
@@ -1494,7 +1489,7 @@
       <c r="B30" t="n">
         <v>91860</v>
       </c>
-      <c r="C30" s="52" t="n">
+      <c r="C30" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
@@ -1525,7 +1520,7 @@
       <c r="B33" t="n">
         <v>91860</v>
       </c>
-      <c r="C33" s="52" t="n">
+      <c r="C33" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D33" t="n">
@@ -1556,7 +1551,7 @@
       <c r="B36" t="n">
         <v>91860</v>
       </c>
-      <c r="C36" s="52" t="n">
+      <c r="C36" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D36" t="n">
@@ -1587,7 +1582,7 @@
       <c r="B39" t="n">
         <v>91860</v>
       </c>
-      <c r="C39" s="52" t="n">
+      <c r="C39" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D39" t="n">
@@ -1610,9 +1605,9 @@
       <c r="C41" s="4" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="53" t="inlineStr">
-        <is>
-          <t>This product is not yet available in game version 4.40 but was added in 5.50.</t>
+      <c r="A42" s="50" t="inlineStr">
+        <is>
+          <t>This product is not yet available in game version 5.00 but was added in 5.50.</t>
         </is>
       </c>
       <c r="C42" s="4" t="n"/>
@@ -4272,7 +4267,7 @@
       </c>
       <c r="D100" s="34" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 4.40 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 5.00 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -12800,7 +12795,7 @@
       </c>
       <c r="D172" s="34" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 4.40 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 5.00 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -14090,7 +14085,7 @@
       </c>
       <c r="D2" s="34" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 4.40 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 5.00 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -14403,7 +14398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14416,7 +14411,7 @@
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
     <col width="5" customWidth="1" min="7" max="7"/>
     <col width="5" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
@@ -14912,41 +14907,199 @@
       <c r="C25" s="4" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="49" t="inlineStr">
+      <c r="A26" s="1" t="inlineStr">
         <is>
           <t>Minotaur Flamethrower (UP_MFIRE)</t>
         </is>
       </c>
-      <c r="B26" s="21" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>Seed</t>
         </is>
       </c>
-      <c r="C26" s="50" t="inlineStr">
+      <c r="C26" s="4" t="inlineStr">
         <is>
           <t>Perfection</t>
         </is>
       </c>
-      <c r="D26" s="51" t="inlineStr">
-        <is>
-          <t>This technology is not yet available in game version 4.40 but was added in 5.00.</t>
-        </is>
-      </c>
-      <c r="E26" s="21" t="n"/>
-      <c r="F26" s="21" t="n"/>
-      <c r="G26" s="21" t="n"/>
-      <c r="H26" s="21" t="n"/>
-      <c r="I26" s="21" t="n"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Damage</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Weapon Power Efficiency</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Impact Fire Duration</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" s="14" t="inlineStr">
+        <is>
+          <t>Supreme Upgrade (4)</t>
+        </is>
+      </c>
+      <c r="B27" s="14" t="inlineStr"/>
+      <c r="C27" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" s="16" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Catalysed Nozzles</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>35809</v>
+      </c>
+      <c r="C28" s="8" t="n">
+        <v>0.995436518192637</v>
+      </c>
+      <c r="D28" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" s="9" t="n">
+        <v>29.8845112323761</v>
+      </c>
+      <c r="F28" s="9" t="n">
+        <v>34.99891757965088</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="17" t="inlineStr">
+        <is>
+          <t>Thermobaric Valves</t>
+        </is>
+      </c>
+      <c r="B29" s="17" t="n">
+        <v>41095</v>
+      </c>
+      <c r="C29" s="18" t="n">
+        <v>0.9906839778356449</v>
+      </c>
+      <c r="D29" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="20" t="n">
+        <v>29.85800504684448</v>
+      </c>
+      <c r="F29" s="20" t="n">
+        <v>34.90149974822998</v>
+      </c>
+      <c r="G29" s="17" t="n"/>
+      <c r="H29" s="17" t="n"/>
+      <c r="I29" s="17" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Superheated Sprayer</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>86542</v>
+      </c>
+      <c r="C30" s="8" t="n">
+        <v>0.9904335068545207</v>
+      </c>
+      <c r="D30" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="9" t="n">
+        <v>29.99722361564636</v>
+      </c>
+      <c r="F30" s="9" t="n">
+        <v>34.75135564804077</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="17" t="inlineStr">
+        <is>
+          <t>Faultless Tubes</t>
+        </is>
+      </c>
+      <c r="B31" s="17" t="n">
+        <v>88680</v>
+      </c>
+      <c r="C31" s="18" t="n">
+        <v>0.9894673369157304</v>
+      </c>
+      <c r="D31" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="20" t="n">
+        <v>29.85437512397766</v>
+      </c>
+      <c r="F31" s="20" t="n">
+        <v>34.87330675125122</v>
+      </c>
+      <c r="G31" s="17" t="n"/>
+      <c r="H31" s="17" t="n"/>
+      <c r="I31" s="17" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Electro-focused Ignition Chamber</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>96019</v>
+      </c>
+      <c r="C32" s="8" t="n">
+        <v>0.6077512309968339</v>
+      </c>
+      <c r="D32" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="9" t="n">
+        <v>20.01542448997498</v>
+      </c>
+      <c r="F32" s="19" t="n">
+        <v>34.99983549118042</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="35" t="inlineStr">
+        <is>
+          <t>Superheated Exhaust</t>
+        </is>
+      </c>
+      <c r="B33" s="35" t="n">
+        <v>46775</v>
+      </c>
+      <c r="C33" s="36" t="n">
+        <v>0.4285695674210536</v>
+      </c>
+      <c r="D33" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="24" t="n">
+        <v>29.99978065490723</v>
+      </c>
+      <c r="F33" s="37" t="n">
+        <v>20.00000476837158</v>
+      </c>
+      <c r="G33" s="35" t="n"/>
+      <c r="H33" s="35" t="n"/>
+      <c r="I33" s="35" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D19:I19"/>
     <mergeCell ref="D10:I10"/>
     <mergeCell ref="D2:I2"/>
-    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D27:I27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>